<commit_message>
[ELAB-414] rework of 'Werkzeuge und Technologien'^2
</commit_message>
<xml_diff>
--- a/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
+++ b/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\tools-und-werkzeuge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{322CF77D-4D02-4070-8386-D909C13EF6CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D5688-C58D-4109-854B-A6F232F98A08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
   </bookViews>
@@ -313,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="145">
   <si>
     <t>Sentry</t>
   </si>
@@ -501,9 +501,6 @@
     <t>Kostenfrei</t>
   </si>
   <si>
-    <t>Deployment</t>
-  </si>
-  <si>
     <t>Prometheus</t>
   </si>
   <si>
@@ -519,9 +516,6 @@
     <t xml:space="preserve"> - Wird standardmäßig von AdBlockern und Firefoxes "Enhanced Tracking Protection" geblockt.</t>
   </si>
   <si>
-    <t>https://s3.cn-north-1.amazonaws.com.cn/market.tingyun.com/solutions/2020Gartner%20APM%E9%AD%94%E5%8A%9B%E8%B1%A1%E9%99%90.pdf</t>
-  </si>
-  <si>
     <t>TrackJS</t>
   </si>
   <si>
@@ -531,49 +525,19 @@
     <t>Session-Replay</t>
   </si>
   <si>
-    <t>https://stackshare.io/exception-monitoring</t>
-  </si>
-  <si>
     <t>FullStory</t>
   </si>
   <si>
     <t xml:space="preserve"> - bieten stark aggreggierte Sichten an</t>
   </si>
   <si>
-    <t>https://stackshare.io/user-feedback-as-a-service</t>
-  </si>
-  <si>
-    <t>Sesson-Replay</t>
-  </si>
-  <si>
     <t>Inspectlet</t>
   </si>
   <si>
     <t xml:space="preserve"> - Entwickler-orientiertes Session-Replay</t>
   </si>
   <si>
-    <t>https://stackshare.io/performance-monitoring</t>
-  </si>
-  <si>
-    <t>APM Gartner</t>
-  </si>
-  <si>
-    <t>APM Stackshare</t>
-  </si>
-  <si>
-    <t>https://link.springer.com/chapter/10.1007/978-3-030-68285-9_39</t>
-  </si>
-  <si>
-    <t>Tracing, Metrics and Logging</t>
-  </si>
-  <si>
-    <t>"Service mesh: Challenges, state of the art, and future research opportunities"</t>
-  </si>
-  <si>
     <t>Fluentd</t>
-  </si>
-  <si>
-    <t>Splunk Enterprise</t>
   </si>
   <si>
     <t xml:space="preserve"> - erlaubt kein direktes Senden von Logs vom Browser aus
@@ -586,9 +550,6 @@
     <t>Technologie</t>
   </si>
   <si>
-    <t>Websupport</t>
-  </si>
-  <si>
     <t>Error-Monitoring</t>
   </si>
   <si>
@@ -610,26 +571,200 @@
     <t>C &amp; OP</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>OP</t>
-  </si>
-  <si>
-    <t>TABLE_BREAK</t>
-  </si>
-  <si>
     <t>TABLE_END</t>
   </si>
   <si>
     <t>bei \mbox{Fehlern}</t>
+  </si>
+  <si>
+    <t>Splunk \mbox{Enterprise}</t>
+  </si>
+  <si>
+    <t>Standardisierung</t>
+  </si>
+  <si>
+    <t>Multifunktional</t>
+  </si>
+  <si>
+    <t>SaaS (z. B. Cloud)</t>
+  </si>
+  <si>
+    <t>Support für Webanw.</t>
+  </si>
+  <si>
+    <t>Zielgruppe</t>
+  </si>
+  <si>
+    <t>geringfügig</t>
+  </si>
+  <si>
+    <t>Fachabteilung, Entwickler</t>
+  </si>
+  <si>
+    <t>Entwickler</t>
+  </si>
+  <si>
+    <t>nein, aber quelloffen</t>
+  </si>
+  <si>
+    <t>Marketing, Fachabteilung, Entwickler</t>
+  </si>
+  <si>
+    <t>Google Analytics</t>
+  </si>
+  <si>
+    <t>Adobe Analytics</t>
+  </si>
+  <si>
+    <t>Papertrail</t>
+  </si>
+  <si>
+    <t>Graylog</t>
+  </si>
+  <si>
+    <t>Gruppe</t>
+  </si>
+  <si>
+    <t>On Premise</t>
+  </si>
+  <si>
+    <t>Metriken</t>
+  </si>
+  <si>
+    <t>Web-Analytics</t>
+  </si>
+  <si>
+    <t>Marketing, Fachabteilung</t>
+  </si>
+  <si>
+    <t>Observability-Plattformen</t>
+  </si>
+  <si>
+    <t>Quellen</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>AppDynamics, Dynatrace, New Relic, Broadcom DX APM, Splunk APM (SignalFX), DataDog</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Gartner Magic Quadrant for Application Performance Monitoring</t>
+  </si>
+  <si>
+    <t>What are the best Performance Monitoring Tools?</t>
+  </si>
+  <si>
+    <t>What are the best Monitoring Tools?</t>
+  </si>
+  <si>
+    <t>What are the best Log Management Tools?</t>
+  </si>
+  <si>
+    <t>What are the best Exception Monitoring Tools?</t>
+  </si>
+  <si>
+    <t>What are the best User-Feedback-as-a-Service Tools?</t>
+  </si>
+  <si>
+    <t>Web and Mobile App Analytics Reviews and Ratings | Gartner Peer Insights</t>
+  </si>
+  <si>
+    <t>Comparison of End-to-End Testing Tools for Microservices: A Case Study</t>
+  </si>
+  <si>
+    <t>Service mesh: Challenges, state of the art, and future research opportunities</t>
+  </si>
+  <si>
+    <t>Multilevel observability in cloud orchestration</t>
+  </si>
+  <si>
+    <t>Webalyt: Implemetation of architecture for capturing web user behaviours with feedback propagation</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>9.</t>
+  </si>
+  <si>
+    <t>10.</t>
+  </si>
+  <si>
+    <t>11.</t>
+  </si>
+  <si>
+    <t>Technologien</t>
+  </si>
+  <si>
+    <t>Inspectlet, FullStory,  LogRocket</t>
+  </si>
+  <si>
+    <t>Fluentd, Prometheus, Zipkin</t>
+  </si>
+  <si>
+    <t>Prometheus, Jaeger, Zipkin, Fluentd</t>
+  </si>
+  <si>
+    <t>Jaeger, Zipkin</t>
+  </si>
+  <si>
+    <t>Elastic Stack, Papertrail, Fluentd, Splunk, Graylog</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Gartner</t>
+  </si>
+  <si>
+    <t>StackShare</t>
+  </si>
+  <si>
+    <t>Literatur</t>
+  </si>
+  <si>
+    <t>Google Analytics, LogRocket, Adobe Analytics</t>
+  </si>
+  <si>
+    <t>Inspectlet, FullStory, LogRocket</t>
+  </si>
+  <si>
+    <t>Sentry, TrackJS, Rollbar</t>
+  </si>
+  <si>
+    <t>New Relic, Elastic Stack, Sentry, Datadog, Prometheus</t>
+  </si>
+  <si>
+    <t>New Relic, Datadog, Dynatrace, AppDynamics, Splunk APM (SignalFX)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -715,6 +850,20 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -790,7 +939,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -902,8 +1051,21 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -918,7 +1080,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -963,23 +1125,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20 % - Akzent3" xfId="1" builtinId="38"/>
@@ -990,7 +1168,77 @@
     <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1314,605 +1562,1339 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FA36FA-A460-4BBC-B832-96B5FC35BB7A}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C18:C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48:P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" style="28"/>
-    <col min="3" max="3" width="11.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.140625" style="28" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.140625" style="28" customWidth="1"/>
-    <col min="13" max="13" width="28.5703125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="28"/>
+    <col min="4" max="4" width="11.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="28" customWidth="1"/>
+    <col min="9" max="9" width="1.140625" style="28" customWidth="1"/>
+    <col min="10" max="10" width="23.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="28" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20" style="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" style="28" customWidth="1"/>
+    <col min="16" max="16" width="34.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.140625" style="28" customWidth="1"/>
+    <col min="18" max="18" width="28.5703125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="46" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" s="44" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>100</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="45" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="45" t="s">
+      <c r="P1" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="46" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+    </row>
+    <row r="3" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="O4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R4" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R5" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="K7" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="R7" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="K8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" s="31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="K11" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M11" s="32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N12" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="O12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P12" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="R12" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="O13" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P13" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="R13" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="K14" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="O14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="R14" s="33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R15" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="45" t="s">
+    </row>
+    <row r="18" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K18" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M18" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N18" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O18" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P18" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="R18" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J19" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M19" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N19" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="O19" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P19" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="R19" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="43" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J22" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K22" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L22" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M22" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N22" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="O22" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P22" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="R22" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J25" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="K25" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L25" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M25" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N25" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="O25" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P25" s="31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J26" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L26" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O26" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P26" s="31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="K27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O27" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P27" s="31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="43" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="K30" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L30" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M30" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N30" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O30" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P30" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R30" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J31" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="K31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L31" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N31" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O31" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P31" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="R31" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="39" t="s">
+    </row>
+    <row r="32" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J32" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="K32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O32" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P32" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="J2" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="M3" s="31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="M4" s="31" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="41" t="s">
+      <c r="R32" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="J5" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" s="41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="41" t="s">
+      <c r="J35" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="K35" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L35" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M35" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N35" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O35" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P35" s="31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E36" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="J6" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="K6" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="M6" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I7" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="J7" s="40" t="s">
-        <v>61</v>
-      </c>
-      <c r="K7" s="41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
+      <c r="J36" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="K36" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L36" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M36" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N36" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O36" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P36" s="31" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B37" s="42" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="B40" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C40" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="50"/>
+      <c r="H40" s="50"/>
+      <c r="J40" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="K40" s="51"/>
+      <c r="L40" s="51"/>
+      <c r="M40" s="51"/>
+      <c r="N40" s="51"/>
+      <c r="O40" s="51"/>
+      <c r="P40" s="51"/>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C41" s="49" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+      <c r="F41" s="49"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="J41" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="K41" s="52"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="52"/>
+      <c r="N41" s="52"/>
+      <c r="O41" s="52"/>
+      <c r="P41" s="52"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C42" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+      <c r="F42" s="49"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="J42" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="K42" s="52"/>
+      <c r="L42" s="52"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="52"/>
+      <c r="O42" s="52"/>
+      <c r="P42" s="52"/>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="G43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="J43" s="52" t="s">
+        <v>143</v>
+      </c>
+      <c r="K43" s="52"/>
+      <c r="L43" s="52"/>
+      <c r="M43" s="52"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="52"/>
+      <c r="P43" s="52"/>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+      <c r="F44" s="49"/>
+      <c r="G44" s="49"/>
+      <c r="H44" s="49"/>
+      <c r="J44" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="K44" s="52"/>
+      <c r="L44" s="52"/>
+      <c r="M44" s="52"/>
+      <c r="N44" s="52"/>
+      <c r="O44" s="52"/>
+      <c r="P44" s="52"/>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49"/>
+      <c r="J45" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="K45" s="52"/>
+      <c r="L45" s="52"/>
+      <c r="M45" s="52"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="52"/>
+      <c r="P45" s="52"/>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" s="49" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+      <c r="J46" s="52" t="s">
+        <v>141</v>
+      </c>
+      <c r="K46" s="52"/>
+      <c r="L46" s="52"/>
+      <c r="M46" s="52"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="52"/>
+      <c r="P46" s="52"/>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="34" t="s">
+        <v>137</v>
+      </c>
+      <c r="C47" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
+      <c r="J47" s="52" t="s">
+        <v>140</v>
+      </c>
+      <c r="K47" s="52"/>
+      <c r="L47" s="52"/>
+      <c r="M47" s="52"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="52"/>
+      <c r="P47" s="52"/>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
+      <c r="J48" s="52" t="s">
+        <v>134</v>
+      </c>
+      <c r="K48" s="52"/>
+      <c r="L48" s="52"/>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="52"/>
+      <c r="P48" s="52"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="49" t="s">
+        <v>117</v>
+      </c>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="49"/>
+      <c r="J49" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="K49" s="52"/>
+      <c r="L49" s="52"/>
+      <c r="M49" s="52"/>
+      <c r="N49" s="52"/>
+      <c r="O49" s="52"/>
+      <c r="P49" s="52"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="J50" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="K50" s="52"/>
+      <c r="L50" s="52"/>
+      <c r="M50" s="52"/>
+      <c r="N50" s="52"/>
+      <c r="O50" s="52"/>
+      <c r="P50" s="52"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C51" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="49"/>
+      <c r="J51" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="K51" s="52"/>
+      <c r="L51" s="52"/>
+      <c r="M51" s="52"/>
+      <c r="N51" s="52"/>
+      <c r="O51" s="52"/>
+      <c r="P51" s="52"/>
+    </row>
+    <row r="61" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="J10" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="M10" s="33" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="K11" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="M11" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="K12" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="M12" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="47" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="K14" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="M14" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I15" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="K15" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="M15" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I16" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="K16" s="41" t="s">
-        <v>96</v>
-      </c>
-      <c r="M16" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I19" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="J19" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>99</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="I20" s="39" t="s">
-        <v>91</v>
-      </c>
-      <c r="J20" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K20" s="30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="J22" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K22" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="M22" s="34" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="41" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="J23" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K23" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="M23" s="31" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="I24" s="41" t="s">
-        <v>92</v>
-      </c>
-      <c r="J24" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="K24" s="35" t="s">
-        <v>94</v>
-      </c>
-      <c r="M24" s="34" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="48" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="B28" s="28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
+      <c r="C61" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="J61" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B31" s="28" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32" s="36" t="s">
+      <c r="K61" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L61" s="30" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" s="28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="28" t="s">
-        <v>72</v>
-      </c>
+      <c r="M61" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="N61" s="30"/>
+      <c r="O61" s="30"/>
+      <c r="P61" s="30"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B11 B13:B24">
+  <mergeCells count="24">
+    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="C45:H45"/>
+    <mergeCell ref="C46:H46"/>
+    <mergeCell ref="C47:H47"/>
+    <mergeCell ref="C48:H48"/>
+    <mergeCell ref="C49:H49"/>
+    <mergeCell ref="J46:P46"/>
+    <mergeCell ref="J47:P47"/>
+    <mergeCell ref="J48:P48"/>
+    <mergeCell ref="J49:P49"/>
+    <mergeCell ref="J50:P50"/>
+    <mergeCell ref="J51:P51"/>
+    <mergeCell ref="J40:P40"/>
+    <mergeCell ref="J41:P41"/>
+    <mergeCell ref="J42:P42"/>
+    <mergeCell ref="J43:P43"/>
+    <mergeCell ref="J44:P44"/>
+    <mergeCell ref="J45:P45"/>
+    <mergeCell ref="C50:H50"/>
+    <mergeCell ref="C51:H51"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="C43:H43"/>
+  </mergeCells>
+  <phoneticPr fontId="13" type="noConversion"/>
+  <conditionalFormatting sqref="C61 C16 C3:C9 C14 C12 C18:C20 C22:C23 C25:C28 C30:C33 C35:C36">
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11:E11 N11:O11 G11:I11">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
@@ -1927,7 +2909,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:J1"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2148,15 +3130,15 @@
       <c r="B9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
       <c r="J9" s="3" t="s">
         <v>19</v>
       </c>
@@ -2242,15 +3224,15 @@
       <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
       <c r="J13" s="3" t="s">
         <v>19</v>
       </c>
@@ -2263,15 +3245,15 @@
       <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="43" t="s">
+      <c r="C14" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
       <c r="J14" s="3" t="s">
         <v>19</v>
       </c>
@@ -2328,15 +3310,15 @@
       <c r="B17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="43"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
       <c r="J17" s="3" t="s">
         <v>19</v>
       </c>
@@ -2349,15 +3331,15 @@
       <c r="B18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="43" t="s">
+      <c r="C18" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
[ELAB-414] rework of 'Werkzeuge und Technologien'^3
</commit_message>
<xml_diff>
--- a/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
+++ b/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\tools-und-werkzeuge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600D5688-C58D-4109-854B-A6F232F98A08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747E1B95-5BA3-45ED-8FF4-BDF2D6BF76F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
+    <workbookView xWindow="14303" yWindow="-98" windowWidth="28995" windowHeight="15945" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
   </bookViews>
   <sheets>
     <sheet name="neue Ansicht" sheetId="2" r:id="rId1"/>
     <sheet name="alte Ansicht" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -313,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="164">
   <si>
     <t>Sentry</t>
   </si>
@@ -565,12 +566,6 @@
     <t>f. begrenzt</t>
   </si>
   <si>
-    <t>unspez.</t>
-  </si>
-  <si>
-    <t>C &amp; OP</t>
-  </si>
-  <si>
     <t>TABLE_END</t>
   </si>
   <si>
@@ -607,9 +602,6 @@
     <t>nein, aber quelloffen</t>
   </si>
   <si>
-    <t>Marketing, Fachabteilung, Entwickler</t>
-  </si>
-  <si>
     <t>Google Analytics</t>
   </si>
   <si>
@@ -634,12 +626,6 @@
     <t>Web-Analytics</t>
   </si>
   <si>
-    <t>Marketing, Fachabteilung</t>
-  </si>
-  <si>
-    <t>Observability-Plattformen</t>
-  </si>
-  <si>
     <t>Quellen</t>
   </si>
   <si>
@@ -757,7 +743,79 @@
     <t>New Relic, Elastic Stack, Sentry, Datadog, Prometheus</t>
   </si>
   <si>
-    <t>New Relic, Datadog, Dynatrace, AppDynamics, Splunk APM (SignalFX)</t>
+    <t>https://www.gartner.com/en/documents/3983892/magic-quadrant-for-application-performance-monitoring</t>
+  </si>
+  <si>
+    <t>https://stackshare.io/performance-monitoring</t>
+  </si>
+  <si>
+    <t>https://stackshare.io/monitoring</t>
+  </si>
+  <si>
+    <t>https://stackshare.io/log-management</t>
+  </si>
+  <si>
+    <t>https://stackshare.io/exception-monitoring</t>
+  </si>
+  <si>
+    <t>https://stackshare.io/user-feedback-as-a-service</t>
+  </si>
+  <si>
+    <t>https://www.gartner.com/reviews/market/web-mobile-app-analytics</t>
+  </si>
+  <si>
+    <t>Li et al.</t>
+  </si>
+  <si>
+    <t>Cristian Martínez et al.</t>
+  </si>
+  <si>
+    <t>Picoreti et al.</t>
+  </si>
+  <si>
+    <t>Filip et al.</t>
+  </si>
+  <si>
+    <t>New Relic, Datadog, Dynatrace, Azure Application Insights, AppDynamics, Splunk APM (SignalFX)</t>
+  </si>
+  <si>
+    <t>Azure Monitor</t>
+  </si>
+  <si>
+    <t>nur Aggregierung</t>
+  </si>
+  <si>
+    <t>Performance-Monitoring</t>
+  </si>
+  <si>
+    <t>Airbrake</t>
+  </si>
+  <si>
+    <t>Bugsnag</t>
+  </si>
+  <si>
+    <t>Raygun</t>
+  </si>
+  <si>
+    <t>gruppiert und bei \mbox{Fehlern}</t>
+  </si>
+  <si>
+    <t>mit Erweiterung</t>
+  </si>
+  <si>
+    <t>Projektmanager, Fachabteilung, Entwickler</t>
+  </si>
+  <si>
+    <t>Projektmanager, Fachabteilung</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Ignore</t>
+  </si>
+  <si>
+    <t>nein, aber teils quelloffen</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1138,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1131,9 +1189,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1149,15 +1204,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20 % - Akzent3" xfId="1" builtinId="38"/>
@@ -1168,7 +1228,28 @@
     <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1562,383 +1643,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FA36FA-A460-4BBC-B832-96B5FC35BB7A}">
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48:P48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="28"/>
-    <col min="4" max="4" width="11.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" style="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="28" customWidth="1"/>
-    <col min="9" max="9" width="1.140625" style="28" customWidth="1"/>
-    <col min="10" max="10" width="23.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="28" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20" style="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.140625" style="28" customWidth="1"/>
-    <col min="16" max="16" width="34.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.140625" style="28" customWidth="1"/>
-    <col min="18" max="18" width="28.5703125" style="28" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="28"/>
+    <col min="5" max="5" width="11.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="28" customWidth="1"/>
+    <col min="10" max="10" width="1.140625" style="28" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="28" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.140625" style="28" customWidth="1"/>
+    <col min="17" max="17" width="34.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="1.140625" style="28" customWidth="1"/>
+    <col min="19" max="19" width="28.5703125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="44" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="45" t="s">
+    <row r="1" spans="1:19" s="43" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="D1" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="E1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="F1" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="G1" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="H1" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="45" t="s">
+      <c r="I1" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="44"/>
+      <c r="K1" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="L1" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="M1" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q1" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
+      <c r="R2" s="46"/>
+      <c r="S2" s="46"/>
+    </row>
+    <row r="3" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="O3" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q3" s="29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="45" t="s">
-        <v>100</v>
-      </c>
-      <c r="M1" s="45" t="s">
-        <v>87</v>
-      </c>
-      <c r="N1" s="45" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="45" t="s">
-        <v>86</v>
-      </c>
-      <c r="P1" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q1" s="45"/>
-      <c r="R1" s="45" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" s="47"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-    </row>
-    <row r="3" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="41" t="s">
+      <c r="P4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="S4" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="37" t="s">
+      <c r="F5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="M3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="N3" s="41" t="s">
+      <c r="L5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="P3" s="29" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N4" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="O4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="P4" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="R4" s="31" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N5" s="39" t="s">
+      <c r="P5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="S5" s="31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="P5" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="R5" s="31" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="G6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="39" t="s">
+      <c r="H6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="39" t="s">
         <v>79</v>
-      </c>
-      <c r="K6" s="38" t="s">
-        <v>60</v>
       </c>
       <c r="L6" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N6" s="38" t="s">
+      <c r="M6" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="O6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="P6" s="31" t="s">
+      <c r="N6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q7" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="S7" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K8" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O8" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K9" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M9" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q9" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="31" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="K7" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="M7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N7" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="O7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="P7" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="R7" s="33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="M8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N8" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="P8" s="31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L11" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="M11" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="36" t="s">
-        <v>16</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>16</v>
@@ -1946,961 +2052,1173 @@
       <c r="E12" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N12" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="O12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="P12" s="31" t="s">
+      <c r="F12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L12" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M12" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O13" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="R12" s="31" t="s">
+      <c r="P13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q13" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="S13" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="31" t="s">
+    <row r="14" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L13" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M13" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N13" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="O13" s="38" t="s">
+      <c r="G14" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="K14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O14" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="P14" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P13" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="R13" s="31" t="s">
+      <c r="Q14" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="S14" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="36" t="s">
+    <row r="15" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="D15" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="E15" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="F15" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="39" t="s">
+      <c r="G15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="K14" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N14" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="O14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="P14" s="31" t="s">
+      <c r="L15" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q15" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="S15" s="33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O16" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="R14" s="33" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+      <c r="P16" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="S16" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K19" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L19" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M19" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O19" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P19" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q19" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="S19" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K20" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O20" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="P20" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q20" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="S20" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="F15" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K15" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L15" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M15" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="R15" s="31" t="s">
+      <c r="B22" s="42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C23" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N23" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O23" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="P23" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q23" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="S23" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="43" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K18" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L18" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M18" s="38" t="s">
+    <row r="24" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O26" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="P26" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N18" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O18" s="38" t="s">
+      <c r="Q26" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K27" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M27" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P18" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="R18" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J19" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L19" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M19" s="38" t="s">
+      <c r="N27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O27" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N19" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="O19" s="38" t="s">
+      <c r="P27" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P19" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="R19" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J22" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K22" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L22" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M22" s="38" t="s">
+      <c r="Q27" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E28" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O28" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N22" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="O22" s="38" t="s">
+      <c r="P28" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q28" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M29" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P22" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="R22" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="43" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J25" s="39" t="s">
+      <c r="N29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O29" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L30" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M30" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N30" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O30" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="P30" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q30" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="D31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="F31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M31" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O31" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P31" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q31" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="K25" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L25" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M25" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N25" s="35" t="s">
-        <v>93</v>
-      </c>
-      <c r="O25" s="38" t="s">
+      <c r="L34" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M34" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P25" s="31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="D26" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J26" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="K26" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L26" s="38" t="s">
+      <c r="N34" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O34" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="M26" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N26" s="38" t="s">
+      <c r="P34" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q34" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="S34" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K35" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L35" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M35" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="O26" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="P26" s="31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="J27" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="K27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N27" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="O27" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="P27" s="31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="43" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="H30" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="K30" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L30" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="M30" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N30" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="O30" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="P30" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="R30" s="31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J31" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="K31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L31" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="M31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N31" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="O31" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="P31" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="R31" s="31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J32" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="K32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N32" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="O32" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="P32" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="R32" s="31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="1:16" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="43" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="D35" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="J35" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="K35" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L35" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="M35" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N35" s="38" t="s">
-        <v>60</v>
+      <c r="N35" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="O35" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P35" s="31" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36" s="39" t="s">
+      <c r="P35" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="J36" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="K36" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L36" s="38" t="s">
-        <v>60</v>
+      <c r="Q35" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="S35" s="31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K36" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L36" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="M36" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="N36" s="38" t="s">
-        <v>60</v>
+      <c r="N36" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="O36" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P36" s="31" t="s">
+      <c r="P36" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q36" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="S36" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" s="42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L39" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M39" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N39" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O39" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P39" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q39" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D40" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="K40" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L40" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M40" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N40" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O40" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P40" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q40" s="29" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C41" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="47"/>
+      <c r="C44" s="47" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" s="51" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B37" s="42" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="48" t="s">
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="51"/>
+      <c r="H44" s="51"/>
+      <c r="I44" s="51"/>
+      <c r="K44" s="50" t="s">
+        <v>125</v>
+      </c>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="E45" s="48"/>
+      <c r="F45" s="48"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="48"/>
+      <c r="I45" s="48"/>
+      <c r="K45" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="49"/>
+      <c r="P45" s="49"/>
+      <c r="Q45" s="49"/>
+      <c r="S45" s="53" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D46" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="B40" s="48" t="s">
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="48"/>
+      <c r="I46" s="48"/>
+      <c r="K46" s="49" t="s">
+        <v>150</v>
+      </c>
+      <c r="L46" s="49"/>
+      <c r="M46" s="49"/>
+      <c r="N46" s="49"/>
+      <c r="O46" s="49"/>
+      <c r="P46" s="49"/>
+      <c r="Q46" s="49"/>
+      <c r="S46" s="53" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>116</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="K47" s="49" t="s">
+        <v>138</v>
+      </c>
+      <c r="L47" s="49"/>
+      <c r="M47" s="49"/>
+      <c r="N47" s="49"/>
+      <c r="O47" s="49"/>
+      <c r="P47" s="49"/>
+      <c r="Q47" s="49"/>
+      <c r="S47" s="53" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>117</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D48" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="K48" s="49" t="s">
+        <v>130</v>
+      </c>
+      <c r="L48" s="49"/>
+      <c r="M48" s="49"/>
+      <c r="N48" s="49"/>
+      <c r="O48" s="49"/>
+      <c r="P48" s="49"/>
+      <c r="Q48" s="49"/>
+      <c r="S48" s="53" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" s="48" t="s">
+        <v>108</v>
+      </c>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="K49" s="49" t="s">
+        <v>137</v>
+      </c>
+      <c r="L49" s="49"/>
+      <c r="M49" s="49"/>
+      <c r="N49" s="49"/>
+      <c r="O49" s="49"/>
+      <c r="P49" s="49"/>
+      <c r="Q49" s="49"/>
+      <c r="S49" s="53" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="D50" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="E50" s="48"/>
+      <c r="F50" s="48"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+      <c r="K50" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="C40" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="50"/>
-      <c r="J40" s="51" t="s">
-        <v>130</v>
-      </c>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="51"/>
-      <c r="P40" s="51"/>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>106</v>
-      </c>
-      <c r="B41" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="C41" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="D41" s="49"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="49"/>
-      <c r="H41" s="49"/>
-      <c r="J41" s="52" t="s">
-        <v>107</v>
-      </c>
-      <c r="K41" s="52"/>
-      <c r="L41" s="52"/>
-      <c r="M41" s="52"/>
-      <c r="N41" s="52"/>
-      <c r="O41" s="52"/>
-      <c r="P41" s="52"/>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="L50" s="49"/>
+      <c r="M50" s="49"/>
+      <c r="N50" s="49"/>
+      <c r="O50" s="49"/>
+      <c r="P50" s="49"/>
+      <c r="Q50" s="49"/>
+      <c r="S50" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>120</v>
       </c>
-      <c r="B42" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="C42" s="49" t="s">
+      <c r="C51" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D51" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="D42" s="49"/>
-      <c r="E42" s="49"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="49"/>
-      <c r="H42" s="49"/>
-      <c r="J42" s="52" t="s">
-        <v>144</v>
-      </c>
-      <c r="K42" s="52"/>
-      <c r="L42" s="52"/>
-      <c r="M42" s="52"/>
-      <c r="N42" s="52"/>
-      <c r="O42" s="52"/>
-      <c r="P42" s="52"/>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="E51" s="48"/>
+      <c r="F51" s="48"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="K51" s="49" t="s">
+        <v>135</v>
+      </c>
+      <c r="L51" s="49"/>
+      <c r="M51" s="49"/>
+      <c r="N51" s="49"/>
+      <c r="O51" s="49"/>
+      <c r="P51" s="49"/>
+      <c r="Q51" s="49"/>
+      <c r="S51" s="53" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>121</v>
       </c>
-      <c r="B43" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="C43" s="49" t="s">
+      <c r="C52" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D52" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="D43" s="49"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="49"/>
-      <c r="H43" s="49"/>
-      <c r="J43" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="K43" s="52"/>
-      <c r="L43" s="52"/>
-      <c r="M43" s="52"/>
-      <c r="N43" s="52"/>
-      <c r="O43" s="52"/>
-      <c r="P43" s="52"/>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="E52" s="48"/>
+      <c r="F52" s="48"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+      <c r="K52" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="L52" s="49"/>
+      <c r="M52" s="49"/>
+      <c r="N52" s="49"/>
+      <c r="O52" s="49"/>
+      <c r="P52" s="49"/>
+      <c r="Q52" s="49"/>
+      <c r="S52" s="28" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>122</v>
       </c>
-      <c r="B44" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="C44" s="49" t="s">
+      <c r="C53" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D53" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="D44" s="49"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49"/>
-      <c r="H44" s="49"/>
-      <c r="J44" s="52" t="s">
-        <v>135</v>
-      </c>
-      <c r="K44" s="52"/>
-      <c r="L44" s="52"/>
-      <c r="M44" s="52"/>
-      <c r="N44" s="52"/>
-      <c r="O44" s="52"/>
-      <c r="P44" s="52"/>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="E53" s="48"/>
+      <c r="F53" s="48"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="48"/>
+      <c r="I53" s="48"/>
+      <c r="K53" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="L53" s="49"/>
+      <c r="M53" s="49"/>
+      <c r="N53" s="49"/>
+      <c r="O53" s="49"/>
+      <c r="P53" s="49"/>
+      <c r="Q53" s="49"/>
+      <c r="S53" s="28" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>123</v>
       </c>
-      <c r="B45" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="49" t="s">
+      <c r="C54" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="49"/>
-      <c r="G45" s="49"/>
-      <c r="H45" s="49"/>
-      <c r="J45" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="K45" s="52"/>
-      <c r="L45" s="52"/>
-      <c r="M45" s="52"/>
-      <c r="N45" s="52"/>
-      <c r="O45" s="52"/>
-      <c r="P45" s="52"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="E54" s="48"/>
+      <c r="F54" s="48"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="K54" s="49" t="s">
+        <v>127</v>
+      </c>
+      <c r="L54" s="49"/>
+      <c r="M54" s="49"/>
+      <c r="N54" s="49"/>
+      <c r="O54" s="49"/>
+      <c r="P54" s="49"/>
+      <c r="Q54" s="49"/>
+      <c r="S54" s="28" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>124</v>
       </c>
-      <c r="B46" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="C46" s="49" t="s">
+      <c r="C55" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="D46" s="49"/>
-      <c r="E46" s="49"/>
-      <c r="F46" s="49"/>
-      <c r="G46" s="49"/>
-      <c r="H46" s="49"/>
-      <c r="J46" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="K46" s="52"/>
-      <c r="L46" s="52"/>
-      <c r="M46" s="52"/>
-      <c r="N46" s="52"/>
-      <c r="O46" s="52"/>
-      <c r="P46" s="52"/>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>125</v>
-      </c>
-      <c r="B47" s="34" t="s">
-        <v>137</v>
-      </c>
-      <c r="C47" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="49"/>
-      <c r="J47" s="52" t="s">
-        <v>140</v>
-      </c>
-      <c r="K47" s="52"/>
-      <c r="L47" s="52"/>
-      <c r="M47" s="52"/>
-      <c r="N47" s="52"/>
-      <c r="O47" s="52"/>
-      <c r="P47" s="52"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="E55" s="48"/>
+      <c r="F55" s="48"/>
+      <c r="G55" s="48"/>
+      <c r="H55" s="48"/>
+      <c r="I55" s="48"/>
+      <c r="K55" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="B48" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="C48" s="49" t="s">
-        <v>116</v>
-      </c>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
-      <c r="G48" s="49"/>
-      <c r="H48" s="49"/>
-      <c r="J48" s="52" t="s">
-        <v>134</v>
-      </c>
-      <c r="K48" s="52"/>
-      <c r="L48" s="52"/>
-      <c r="M48" s="52"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="52"/>
-      <c r="P48" s="52"/>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>127</v>
-      </c>
-      <c r="B49" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="C49" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="D49" s="49"/>
-      <c r="E49" s="49"/>
-      <c r="F49" s="49"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="49"/>
-      <c r="J49" s="52" t="s">
-        <v>133</v>
-      </c>
-      <c r="K49" s="52"/>
-      <c r="L49" s="52"/>
-      <c r="M49" s="52"/>
-      <c r="N49" s="52"/>
-      <c r="O49" s="52"/>
-      <c r="P49" s="52"/>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>128</v>
-      </c>
-      <c r="B50" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="C50" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="D50" s="49"/>
-      <c r="E50" s="49"/>
-      <c r="F50" s="49"/>
-      <c r="G50" s="49"/>
-      <c r="H50" s="49"/>
-      <c r="J50" s="52" t="s">
-        <v>132</v>
-      </c>
-      <c r="K50" s="52"/>
-      <c r="L50" s="52"/>
-      <c r="M50" s="52"/>
-      <c r="N50" s="52"/>
-      <c r="O50" s="52"/>
-      <c r="P50" s="52"/>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>129</v>
-      </c>
-      <c r="B51" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="C51" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="D51" s="49"/>
-      <c r="E51" s="49"/>
-      <c r="F51" s="49"/>
-      <c r="G51" s="49"/>
-      <c r="H51" s="49"/>
-      <c r="J51" s="52" t="s">
-        <v>131</v>
-      </c>
-      <c r="K51" s="52"/>
-      <c r="L51" s="52"/>
-      <c r="M51" s="52"/>
-      <c r="N51" s="52"/>
-      <c r="O51" s="52"/>
-      <c r="P51" s="52"/>
-    </row>
-    <row r="61" spans="1:16" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="31" t="s">
+      <c r="L55" s="49"/>
+      <c r="M55" s="49"/>
+      <c r="N55" s="49"/>
+      <c r="O55" s="49"/>
+      <c r="P55" s="49"/>
+      <c r="Q55" s="49"/>
+      <c r="S55" s="34" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="65" spans="3:17" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C61" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="D61" s="39" t="s">
+      <c r="D65" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="E61" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G61" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="J61" s="37" t="s">
+      <c r="F65" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H65" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K65" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="K61" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L61" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="M61" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="N61" s="30"/>
-      <c r="O61" s="30"/>
-      <c r="P61" s="30"/>
+      <c r="L65" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M65" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N65" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O65" s="30"/>
+      <c r="P65" s="30"/>
+      <c r="Q65" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C44:H44"/>
-    <mergeCell ref="C45:H45"/>
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="C47:H47"/>
-    <mergeCell ref="C48:H48"/>
-    <mergeCell ref="C49:H49"/>
-    <mergeCell ref="J46:P46"/>
-    <mergeCell ref="J47:P47"/>
-    <mergeCell ref="J48:P48"/>
-    <mergeCell ref="J49:P49"/>
-    <mergeCell ref="J50:P50"/>
-    <mergeCell ref="J51:P51"/>
-    <mergeCell ref="J40:P40"/>
-    <mergeCell ref="J41:P41"/>
-    <mergeCell ref="J42:P42"/>
-    <mergeCell ref="J43:P43"/>
-    <mergeCell ref="J44:P44"/>
-    <mergeCell ref="J45:P45"/>
-    <mergeCell ref="C50:H50"/>
-    <mergeCell ref="C51:H51"/>
-    <mergeCell ref="C40:H40"/>
-    <mergeCell ref="C41:H41"/>
-    <mergeCell ref="C42:H42"/>
-    <mergeCell ref="C43:H43"/>
+    <mergeCell ref="D54:I54"/>
+    <mergeCell ref="D55:I55"/>
+    <mergeCell ref="D44:I44"/>
+    <mergeCell ref="D45:I45"/>
+    <mergeCell ref="D46:I46"/>
+    <mergeCell ref="D47:I47"/>
+    <mergeCell ref="K54:Q54"/>
+    <mergeCell ref="K55:Q55"/>
+    <mergeCell ref="K44:Q44"/>
+    <mergeCell ref="K45:Q45"/>
+    <mergeCell ref="K46:Q46"/>
+    <mergeCell ref="K47:Q47"/>
+    <mergeCell ref="K48:Q48"/>
+    <mergeCell ref="K49:Q49"/>
+    <mergeCell ref="D53:I53"/>
+    <mergeCell ref="K50:Q50"/>
+    <mergeCell ref="K51:Q51"/>
+    <mergeCell ref="K52:Q52"/>
+    <mergeCell ref="K53:Q53"/>
+    <mergeCell ref="D48:I48"/>
+    <mergeCell ref="D49:I49"/>
+    <mergeCell ref="D50:I50"/>
+    <mergeCell ref="D51:I51"/>
+    <mergeCell ref="D52:I52"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="C61 C16 C3:C9 C14 C12 C18:C20 C22:C23 C25:C28 C30:C33 C35:C36">
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+  <conditionalFormatting sqref="D65 D17 D15 D13 D19:D21 D23:D24 D26:D28 D34:D37 D3:D10 D32">
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+  <conditionalFormatting sqref="D37">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+  <conditionalFormatting sqref="D11">
+    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+  <conditionalFormatting sqref="D18">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+  <conditionalFormatting sqref="H12:J12">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:E11 N11:O11 G11:I11">
+  <conditionalFormatting sqref="D22">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
+  <conditionalFormatting sqref="D33">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="D38">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
+  <conditionalFormatting sqref="D16">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
+  <conditionalFormatting sqref="D12">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+  <conditionalFormatting sqref="D30">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="S45" r:id="rId1" xr:uid="{2F2AC83B-E3C5-42BC-A8AB-1C13D82BD690}"/>
+    <hyperlink ref="S46" r:id="rId2" xr:uid="{0FBD89B3-32F8-40AC-842E-8AD0D2B6C2F3}"/>
+    <hyperlink ref="S47" r:id="rId3" xr:uid="{620B8347-8EF9-46A1-BCD7-CC9AC99A521B}"/>
+    <hyperlink ref="S48" r:id="rId4" xr:uid="{52BB097F-4337-40BC-8429-4EAACC609E96}"/>
+    <hyperlink ref="S49" r:id="rId5" xr:uid="{86D7D8D2-4A6F-429E-82A4-8F3837AB5B83}"/>
+    <hyperlink ref="S50" r:id="rId6" xr:uid="{04E81D6C-FFE2-491C-ADE3-C5A4302B59D8}"/>
+    <hyperlink ref="S51" r:id="rId7" xr:uid="{01914F05-ABA5-4B96-8522-4554F7DCD64D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -3130,15 +3448,15 @@
       <c r="B9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="40" t="s">
+      <c r="C9" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
       <c r="J9" s="3" t="s">
         <v>19</v>
       </c>
@@ -3224,15 +3542,15 @@
       <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
       <c r="J13" s="3" t="s">
         <v>19</v>
       </c>
@@ -3245,15 +3563,15 @@
       <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
       <c r="J14" s="3" t="s">
         <v>19</v>
       </c>
@@ -3310,15 +3628,15 @@
       <c r="B17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
       <c r="J17" s="3" t="s">
         <v>19</v>
       </c>
@@ -3331,15 +3649,15 @@
       <c r="B18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
       <c r="J18" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
[ELAB-414] rework of 'Werkzeuge und Technologien'^5
</commit_message>
<xml_diff>
--- a/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
+++ b/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\tools-und-werkzeuge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747E1B95-5BA3-45ED-8FF4-BDF2D6BF76F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749F9378-531A-4797-AD6E-6CF58FE59B44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-98" windowWidth="28995" windowHeight="15945" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
   </bookViews>
   <sheets>
     <sheet name="neue Ansicht" sheetId="2" r:id="rId1"/>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="166">
   <si>
     <t>Sentry</t>
   </si>
@@ -620,9 +620,6 @@
     <t>On Premise</t>
   </si>
   <si>
-    <t>Metriken</t>
-  </si>
-  <si>
     <t>Web-Analytics</t>
   </si>
   <si>
@@ -782,9 +779,6 @@
     <t>Azure Monitor</t>
   </si>
   <si>
-    <t>nur Aggregierung</t>
-  </si>
-  <si>
     <t>Performance-Monitoring</t>
   </si>
   <si>
@@ -797,12 +791,6 @@
     <t>Raygun</t>
   </si>
   <si>
-    <t>gruppiert und bei \mbox{Fehlern}</t>
-  </si>
-  <si>
-    <t>mit Erweiterung</t>
-  </si>
-  <si>
     <t>Projektmanager, Fachabteilung, Entwickler</t>
   </si>
   <si>
@@ -816,6 +804,24 @@
   </si>
   <si>
     <t>nein, aber teils quelloffen</t>
+  </si>
+  <si>
+    <t>mit Erw.</t>
+  </si>
+  <si>
+    <t>nur Agg.</t>
+  </si>
+  <si>
+    <t>grupp. und bei \mbox{Fehlern}</t>
+  </si>
+  <si>
+    <t>Log-Plattform</t>
+  </si>
+  <si>
+    <t>Tracing-Plattform</t>
+  </si>
+  <si>
+    <t>Error-Tracking</t>
   </si>
 </sst>
 </file>
@@ -1228,21 +1234,7 @@
     <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill>
@@ -1643,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FA36FA-A460-4BBC-B832-96B5FC35BB7A}">
-  <dimension ref="A1:S65"/>
+  <dimension ref="A1:S63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,7 +1669,7 @@
         <v>96</v>
       </c>
       <c r="B1" s="54" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C1" s="44" t="s">
         <v>74</v>
@@ -1729,10 +1721,10 @@
     </row>
     <row r="2" spans="1:19" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -1759,14 +1751,14 @@
       <c r="D3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="39" t="s">
         <v>73</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>9</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H3" s="30" t="s">
         <v>9</v>
@@ -1790,7 +1782,7 @@
         <v>9</v>
       </c>
       <c r="Q3" s="29" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -1831,7 +1823,7 @@
         <v>9</v>
       </c>
       <c r="Q4" s="29" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="S4" s="31" t="s">
         <v>62</v>
@@ -1875,7 +1867,7 @@
         <v>9</v>
       </c>
       <c r="Q5" s="29" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="S5" s="31" t="s">
         <v>63</v>
@@ -1916,7 +1908,7 @@
         <v>9</v>
       </c>
       <c r="Q6" s="29" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2000,7 +1992,7 @@
     </row>
     <row r="9" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C9" s="31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>9</v>
@@ -2036,53 +2028,47 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D12" s="36" t="s">
+    <row r="10" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K12" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="L12" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="M12" s="38" t="s">
+      <c r="M10" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O12" s="38" t="s">
+      <c r="O10" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="P10" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P12" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q12" s="31" t="s">
+      <c r="Q10" s="31" t="s">
         <v>89</v>
+      </c>
+      <c r="S10" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="42" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C13" s="31" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>16</v>
@@ -2096,20 +2082,20 @@
       <c r="G13" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K13" s="32" t="s">
-        <v>9</v>
+      <c r="K13" s="39" t="s">
+        <v>79</v>
       </c>
       <c r="L13" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="32" t="s">
-        <v>9</v>
+      <c r="M13" s="38" t="s">
+        <v>60</v>
       </c>
       <c r="N13" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O13" s="35" t="s">
-        <v>91</v>
+      <c r="O13" s="38" t="s">
+        <v>60</v>
       </c>
       <c r="P13" s="32" t="s">
         <v>9</v>
@@ -2117,16 +2103,22 @@
       <c r="Q13" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="S13" s="31" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="14" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>152</v>
+        <v>3</v>
+      </c>
+      <c r="D14" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="K14" s="32" t="s">
         <v>9</v>
@@ -2143,11 +2135,11 @@
       <c r="O14" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="P14" s="38" t="s">
-        <v>60</v>
+      <c r="P14" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="Q14" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S14" s="31" t="s">
         <v>35</v>
@@ -2155,22 +2147,13 @@
     </row>
     <row r="15" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C15" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D15" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K15" s="39" t="s">
-        <v>79</v>
+        <v>71</v>
+      </c>
+      <c r="G15" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="K15" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="L15" s="36" t="s">
         <v>16</v>
@@ -2181,22 +2164,22 @@
       <c r="N15" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O15" s="38" t="s">
+      <c r="O15" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="P15" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P15" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="Q15" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="S15" s="33" t="s">
-        <v>72</v>
+        <v>90</v>
+      </c>
+      <c r="S15" s="31" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C16" s="31" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>16</v>
@@ -2210,8 +2193,8 @@
       <c r="G16" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="32" t="s">
-        <v>9</v>
+      <c r="K16" s="39" t="s">
+        <v>79</v>
       </c>
       <c r="L16" s="36" t="s">
         <v>16</v>
@@ -2222,60 +2205,69 @@
       <c r="N16" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O16" s="35" t="s">
+      <c r="O16" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P16" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q16" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="S16" s="33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="M17" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N17" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O17" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="P16" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q16" s="31" t="s">
+      <c r="P17" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q17" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="S16" s="31" t="s">
+      <c r="S17" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="H19" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L19" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="M19" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N19" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="O19" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="P19" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q19" s="31" t="s">
-        <v>90</v>
-      </c>
-      <c r="S19" s="31" t="s">
-        <v>35</v>
+    <row r="18" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="42" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H20" s="32" t="s">
         <v>9</v>
@@ -2292,8 +2284,8 @@
       <c r="N20" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="O20" s="35" t="s">
-        <v>91</v>
+      <c r="O20" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="P20" s="38" t="s">
         <v>60</v>
@@ -2305,56 +2297,111 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="42" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="42" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="D23" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K23" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L23" s="36" t="s">
+    <row r="21" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C21" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K21" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L21" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M23" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N23" s="38" t="s">
+      <c r="M21" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N21" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="O23" s="35" t="s">
+      <c r="O21" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="P23" s="38" t="s">
+      <c r="P21" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q23" s="31" t="s">
+      <c r="Q21" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="S21" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="42" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L24" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M24" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="P24" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q24" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="S23" s="31" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="42" t="s">
-        <v>75</v>
+    </row>
+    <row r="25" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K25" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L25" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M25" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N25" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O25" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P25" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q25" s="31" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="31" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="E26" s="35" t="s">
         <v>81</v>
@@ -2362,8 +2409,8 @@
       <c r="F26" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K26" s="39" t="s">
-        <v>79</v>
+      <c r="K26" s="35" t="s">
+        <v>78</v>
       </c>
       <c r="L26" s="32" t="s">
         <v>9</v>
@@ -2374,11 +2421,11 @@
       <c r="N26" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O26" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="P26" s="38" t="s">
+      <c r="O26" s="38" t="s">
         <v>60</v>
+      </c>
+      <c r="P26" s="39" t="s">
+        <v>23</v>
       </c>
       <c r="Q26" s="31" t="s">
         <v>89</v>
@@ -2386,10 +2433,10 @@
     </row>
     <row r="27" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="E27" s="35" t="s">
-        <v>81</v>
+        <v>152</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="F27" s="32" t="s">
         <v>9</v>
@@ -2409,8 +2456,8 @@
       <c r="O27" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P27" s="38" t="s">
-        <v>60</v>
+      <c r="P27" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="Q27" s="31" t="s">
         <v>89</v>
@@ -2418,10 +2465,7 @@
     </row>
     <row r="28" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="E28" s="35" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="F28" s="32" t="s">
         <v>9</v>
@@ -2438,11 +2482,11 @@
       <c r="N28" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O28" s="38" t="s">
+      <c r="O28" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="P28" s="38" t="s">
         <v>60</v>
-      </c>
-      <c r="P28" s="39" t="s">
-        <v>23</v>
       </c>
       <c r="Q28" s="31" t="s">
         <v>89</v>
@@ -2455,6 +2499,9 @@
       <c r="D29" s="32" t="s">
         <v>9</v>
       </c>
+      <c r="E29" s="39" t="s">
+        <v>162</v>
+      </c>
       <c r="F29" s="32" t="s">
         <v>9</v>
       </c>
@@ -2480,84 +2527,99 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="31" t="s">
+    <row r="30" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M32" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="N32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O32" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P32" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q32" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="F30" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K30" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="L30" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M30" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N30" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O30" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="P30" s="38" t="s">
+      <c r="S32" s="31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C33" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="I33" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K33" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="L33" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M33" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q30" s="31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C31" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="39" t="s">
-        <v>157</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K31" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="L31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M31" s="38" t="s">
+      <c r="N33" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O33" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O31" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="P31" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q31" s="31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="42" t="s">
-        <v>66</v>
+      <c r="P33" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q33" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="S33" s="31" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="31" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="E34" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F34" s="39" t="s">
+      <c r="F34" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="39" t="s">
         <v>23</v>
       </c>
       <c r="I34" s="32" t="s">
@@ -2569,8 +2631,8 @@
       <c r="L34" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="M34" s="38" t="s">
-        <v>60</v>
+      <c r="M34" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="N34" s="32" t="s">
         <v>9</v>
@@ -2581,211 +2643,188 @@
       <c r="P34" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Q34" s="29" t="s">
-        <v>159</v>
+      <c r="Q34" s="31" t="s">
+        <v>89</v>
       </c>
       <c r="S34" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="31" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="39" t="s">
+    <row r="35" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="42" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K35" s="39" t="s">
+      <c r="E37" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="L35" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M35" s="38" t="s">
+      <c r="L37" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M37" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N35" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O35" s="38" t="s">
+      <c r="N37" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O37" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P35" s="39" t="s">
+      <c r="P37" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q37" s="29" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Q35" s="29" t="s">
-        <v>159</v>
-      </c>
-      <c r="S35" s="31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="39" t="s">
+      <c r="E38" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="I36" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K36" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="L36" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M36" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N36" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O36" s="38" t="s">
+      <c r="K38" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="L38" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M38" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P36" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q36" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="S36" s="31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="42" t="s">
+      <c r="N38" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O38" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="P38" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q38" s="29" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C39" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="B38" s="42" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D39" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="F39" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="K39" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="L39" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M39" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="N39" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O39" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="P39" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q39" s="29" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D40" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="F40" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="K40" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="L40" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M40" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="N40" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O40" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="P40" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q40" s="29" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C41" s="41" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="47" t="s">
+      <c r="B42" s="47"/>
+      <c r="C42" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="D42" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="K42" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="L42" s="50"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="50"/>
+      <c r="P42" s="50"/>
+      <c r="Q42" s="50"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>100</v>
       </c>
-      <c r="B44" s="47"/>
-      <c r="C44" s="47" t="s">
+      <c r="C43" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="D44" s="51" t="s">
+      <c r="D43" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="51"/>
-      <c r="I44" s="51"/>
-      <c r="K44" s="50" t="s">
-        <v>125</v>
-      </c>
-      <c r="L44" s="50"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="50"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="50"/>
+      <c r="E43" s="48"/>
+      <c r="F43" s="48"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="K43" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="L43" s="49"/>
+      <c r="M43" s="49"/>
+      <c r="N43" s="49"/>
+      <c r="O43" s="49"/>
+      <c r="P43" s="49"/>
+      <c r="Q43" s="49"/>
+      <c r="S43" s="53" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>114</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="E44" s="48"/>
+      <c r="F44" s="48"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="K44" s="49" t="s">
+        <v>149</v>
+      </c>
+      <c r="L44" s="49"/>
+      <c r="M44" s="49"/>
+      <c r="N44" s="49"/>
+      <c r="O44" s="49"/>
+      <c r="P44" s="49"/>
+      <c r="Q44" s="49"/>
+      <c r="S44" s="53" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="C45" s="34" t="s">
         <v>132</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E45" s="48"/>
       <c r="F45" s="48"/>
@@ -2793,7 +2832,7 @@
       <c r="H45" s="48"/>
       <c r="I45" s="48"/>
       <c r="K45" s="49" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
       <c r="L45" s="49"/>
       <c r="M45" s="49"/>
@@ -2802,18 +2841,18 @@
       <c r="P45" s="49"/>
       <c r="Q45" s="49"/>
       <c r="S45" s="53" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E46" s="48"/>
       <c r="F46" s="48"/>
@@ -2821,7 +2860,7 @@
       <c r="H46" s="48"/>
       <c r="I46" s="48"/>
       <c r="K46" s="49" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="L46" s="49"/>
       <c r="M46" s="49"/>
@@ -2830,18 +2869,18 @@
       <c r="P46" s="49"/>
       <c r="Q46" s="49"/>
       <c r="S46" s="53" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E47" s="48"/>
       <c r="F47" s="48"/>
@@ -2849,7 +2888,7 @@
       <c r="H47" s="48"/>
       <c r="I47" s="48"/>
       <c r="K47" s="49" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="L47" s="49"/>
       <c r="M47" s="49"/>
@@ -2858,18 +2897,18 @@
       <c r="P47" s="49"/>
       <c r="Q47" s="49"/>
       <c r="S47" s="53" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C48" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E48" s="48"/>
       <c r="F48" s="48"/>
@@ -2877,7 +2916,7 @@
       <c r="H48" s="48"/>
       <c r="I48" s="48"/>
       <c r="K48" s="49" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="L48" s="49"/>
       <c r="M48" s="49"/>
@@ -2886,18 +2925,18 @@
       <c r="P48" s="49"/>
       <c r="Q48" s="49"/>
       <c r="S48" s="53" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E49" s="48"/>
       <c r="F49" s="48"/>
@@ -2905,7 +2944,7 @@
       <c r="H49" s="48"/>
       <c r="I49" s="48"/>
       <c r="K49" s="49" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="L49" s="49"/>
       <c r="M49" s="49"/>
@@ -2914,18 +2953,18 @@
       <c r="P49" s="49"/>
       <c r="Q49" s="49"/>
       <c r="S49" s="53" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C50" s="34" t="s">
         <v>133</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E50" s="48"/>
       <c r="F50" s="48"/>
@@ -2933,7 +2972,7 @@
       <c r="H50" s="48"/>
       <c r="I50" s="48"/>
       <c r="K50" s="49" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="L50" s="49"/>
       <c r="M50" s="49"/>
@@ -2941,19 +2980,19 @@
       <c r="O50" s="49"/>
       <c r="P50" s="49"/>
       <c r="Q50" s="49"/>
-      <c r="S50" s="53" t="s">
-        <v>144</v>
+      <c r="S50" s="28" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D51" s="48" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E51" s="48"/>
       <c r="F51" s="48"/>
@@ -2961,7 +3000,7 @@
       <c r="H51" s="48"/>
       <c r="I51" s="48"/>
       <c r="K51" s="49" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="L51" s="49"/>
       <c r="M51" s="49"/>
@@ -2969,19 +3008,19 @@
       <c r="O51" s="49"/>
       <c r="P51" s="49"/>
       <c r="Q51" s="49"/>
-      <c r="S51" s="53" t="s">
+      <c r="S51" s="28" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C52" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D52" s="48" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E52" s="48"/>
       <c r="F52" s="48"/>
@@ -2989,7 +3028,7 @@
       <c r="H52" s="48"/>
       <c r="I52" s="48"/>
       <c r="K52" s="49" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="L52" s="49"/>
       <c r="M52" s="49"/>
@@ -3003,13 +3042,13 @@
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E53" s="48"/>
       <c r="F53" s="48"/>
@@ -3017,7 +3056,7 @@
       <c r="H53" s="48"/>
       <c r="I53" s="48"/>
       <c r="K53" s="49" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="L53" s="49"/>
       <c r="M53" s="49"/>
@@ -3025,197 +3064,136 @@
       <c r="O53" s="49"/>
       <c r="P53" s="49"/>
       <c r="Q53" s="49"/>
-      <c r="S53" s="28" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>123</v>
-      </c>
-      <c r="C54" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="D54" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="E54" s="48"/>
-      <c r="F54" s="48"/>
-      <c r="G54" s="48"/>
-      <c r="H54" s="48"/>
-      <c r="I54" s="48"/>
-      <c r="K54" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="L54" s="49"/>
-      <c r="M54" s="49"/>
-      <c r="N54" s="49"/>
-      <c r="O54" s="49"/>
-      <c r="P54" s="49"/>
-      <c r="Q54" s="49"/>
-      <c r="S54" s="28" t="s">
+      <c r="S53" s="34" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>124</v>
-      </c>
-      <c r="C55" s="34" t="s">
-        <v>134</v>
-      </c>
-      <c r="D55" s="48" t="s">
-        <v>114</v>
-      </c>
-      <c r="E55" s="48"/>
-      <c r="F55" s="48"/>
-      <c r="G55" s="48"/>
-      <c r="H55" s="48"/>
-      <c r="I55" s="48"/>
-      <c r="K55" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="L55" s="49"/>
-      <c r="M55" s="49"/>
-      <c r="N55" s="49"/>
-      <c r="O55" s="49"/>
-      <c r="P55" s="49"/>
-      <c r="Q55" s="49"/>
-      <c r="S55" s="34" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="65" spans="3:17" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="31" t="s">
+    <row r="63" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="D65" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="39" t="s">
+      <c r="D63" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F65" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G65" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="H65" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K65" s="37" t="s">
+      <c r="F63" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H63" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K63" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="L65" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M65" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N65" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O65" s="30"/>
-      <c r="P65" s="30"/>
-      <c r="Q65" s="30"/>
+      <c r="L63" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M63" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N63" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O63" s="30"/>
+      <c r="P63" s="30"/>
+      <c r="Q63" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D54:I54"/>
-    <mergeCell ref="D55:I55"/>
+    <mergeCell ref="D52:I52"/>
+    <mergeCell ref="D53:I53"/>
+    <mergeCell ref="D42:I42"/>
+    <mergeCell ref="D43:I43"/>
     <mergeCell ref="D44:I44"/>
     <mergeCell ref="D45:I45"/>
-    <mergeCell ref="D46:I46"/>
-    <mergeCell ref="D47:I47"/>
-    <mergeCell ref="K54:Q54"/>
-    <mergeCell ref="K55:Q55"/>
+    <mergeCell ref="K52:Q52"/>
+    <mergeCell ref="K53:Q53"/>
+    <mergeCell ref="K42:Q42"/>
+    <mergeCell ref="K43:Q43"/>
     <mergeCell ref="K44:Q44"/>
     <mergeCell ref="K45:Q45"/>
     <mergeCell ref="K46:Q46"/>
     <mergeCell ref="K47:Q47"/>
+    <mergeCell ref="D51:I51"/>
     <mergeCell ref="K48:Q48"/>
     <mergeCell ref="K49:Q49"/>
-    <mergeCell ref="D53:I53"/>
     <mergeCell ref="K50:Q50"/>
     <mergeCell ref="K51:Q51"/>
-    <mergeCell ref="K52:Q52"/>
-    <mergeCell ref="K53:Q53"/>
+    <mergeCell ref="D46:I46"/>
+    <mergeCell ref="D47:I47"/>
     <mergeCell ref="D48:I48"/>
     <mergeCell ref="D49:I49"/>
     <mergeCell ref="D50:I50"/>
-    <mergeCell ref="D51:I51"/>
-    <mergeCell ref="D52:I52"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="D65 D17 D15 D13 D19:D21 D23:D24 D26:D28 D34:D37 D3:D10 D32">
-    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
+  <conditionalFormatting sqref="D63 D18 D16 D14 D24:D26 D32:D35 D30 D20:D22 D3:D11">
+    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D37">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+  <conditionalFormatting sqref="D35">
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="cellIs" dxfId="10" priority="13" operator="equal">
+  <conditionalFormatting sqref="D12">
+    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D18">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+  <conditionalFormatting sqref="D19">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:J12">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+  <conditionalFormatting sqref="H13:J13">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
-      <formula>"ja"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
+  <conditionalFormatting sqref="D23">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="D31">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
+  <conditionalFormatting sqref="D17">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
+  <conditionalFormatting sqref="D13">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D30">
+  <conditionalFormatting sqref="D28">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="S45" r:id="rId1" xr:uid="{2F2AC83B-E3C5-42BC-A8AB-1C13D82BD690}"/>
-    <hyperlink ref="S46" r:id="rId2" xr:uid="{0FBD89B3-32F8-40AC-842E-8AD0D2B6C2F3}"/>
-    <hyperlink ref="S47" r:id="rId3" xr:uid="{620B8347-8EF9-46A1-BCD7-CC9AC99A521B}"/>
-    <hyperlink ref="S48" r:id="rId4" xr:uid="{52BB097F-4337-40BC-8429-4EAACC609E96}"/>
-    <hyperlink ref="S49" r:id="rId5" xr:uid="{86D7D8D2-4A6F-429E-82A4-8F3837AB5B83}"/>
-    <hyperlink ref="S50" r:id="rId6" xr:uid="{04E81D6C-FFE2-491C-ADE3-C5A4302B59D8}"/>
-    <hyperlink ref="S51" r:id="rId7" xr:uid="{01914F05-ABA5-4B96-8522-4554F7DCD64D}"/>
+    <hyperlink ref="S43" r:id="rId1" xr:uid="{2F2AC83B-E3C5-42BC-A8AB-1C13D82BD690}"/>
+    <hyperlink ref="S44" r:id="rId2" xr:uid="{0FBD89B3-32F8-40AC-842E-8AD0D2B6C2F3}"/>
+    <hyperlink ref="S45" r:id="rId3" xr:uid="{620B8347-8EF9-46A1-BCD7-CC9AC99A521B}"/>
+    <hyperlink ref="S46" r:id="rId4" xr:uid="{52BB097F-4337-40BC-8429-4EAACC609E96}"/>
+    <hyperlink ref="S47" r:id="rId5" xr:uid="{86D7D8D2-4A6F-429E-82A4-8F3837AB5B83}"/>
+    <hyperlink ref="S48" r:id="rId6" xr:uid="{04E81D6C-FFE2-491C-ADE3-C5A4302B59D8}"/>
+    <hyperlink ref="S49" r:id="rId7" xr:uid="{01914F05-ABA5-4B96-8522-4554F7DCD64D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>

</xml_diff>

<commit_message>
[ELAB-414] rework of 'Werkzeuge und Technologien'^6
</commit_message>
<xml_diff>
--- a/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
+++ b/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\tools-und-werkzeuge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749F9378-531A-4797-AD6E-6CF58FE59B44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB94005-2355-4F22-A5B5-B0F55042542A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
   </bookViews>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="170">
   <si>
     <t>Sentry</t>
   </si>
@@ -779,9 +779,6 @@
     <t>Azure Monitor</t>
   </si>
   <si>
-    <t>Performance-Monitoring</t>
-  </si>
-  <si>
     <t>Airbrake</t>
   </si>
   <si>
@@ -822,6 +819,21 @@
   </si>
   <si>
     <t>Error-Tracking</t>
+  </si>
+  <si>
+    <t>ASM</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>mögl.</t>
+  </si>
+  <si>
+    <t>APM-Plattform</t>
+  </si>
+  <si>
+    <t>Session-Replay-Dienst</t>
   </si>
 </sst>
 </file>
@@ -1207,9 +1219,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1224,6 +1233,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20 % - Akzent3" xfId="1" builtinId="38"/>
@@ -1234,7 +1246,70 @@
     <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1635,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FA36FA-A460-4BBC-B832-96B5FC35BB7A}">
-  <dimension ref="A1:S63"/>
+  <dimension ref="A1:T63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37:E38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,85 +1721,89 @@
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="2.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="28"/>
-    <col min="5" max="5" width="11.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" style="28" customWidth="1"/>
-    <col min="10" max="10" width="1.140625" style="28" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" style="28" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="28" customWidth="1"/>
-    <col min="13" max="13" width="10.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20" style="28" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" style="28" customWidth="1"/>
-    <col min="17" max="17" width="34.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="1.140625" style="28" customWidth="1"/>
-    <col min="19" max="19" width="28.5703125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="28" customWidth="1"/>
+    <col min="5" max="5" width="8.140625" style="28" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="28" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="28" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="28" customWidth="1"/>
+    <col min="11" max="11" width="1.140625" style="28" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" style="28" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" style="28" customWidth="1"/>
+    <col min="18" max="18" width="34.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="1.140625" style="28" customWidth="1"/>
+    <col min="20" max="20" width="28.5703125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="43" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="43" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="54" t="s">
-        <v>158</v>
+      <c r="B1" s="53" t="s">
+        <v>157</v>
       </c>
       <c r="C1" s="44" t="s">
         <v>74</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>4</v>
+        <v>166</v>
       </c>
       <c r="E1" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="G1" s="44" t="s">
         <v>75</v>
-      </c>
-      <c r="G1" s="44" t="s">
-        <v>76</v>
       </c>
       <c r="H1" s="44" t="s">
         <v>34</v>
       </c>
       <c r="I1" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="J1" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="44"/>
+      <c r="L1" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="M1" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="M1" s="44" t="s">
+      <c r="N1" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="N1" s="44" t="s">
+      <c r="O1" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="O1" s="44" t="s">
+      <c r="P1" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="Q1" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="Q1" s="44" t="s">
+      <c r="R1" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44" t="s">
+      <c r="S1" s="44"/>
+      <c r="T1" s="44" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="45" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -1743,261 +1822,280 @@
       <c r="Q2" s="46"/>
       <c r="R2" s="46"/>
       <c r="S2" s="46"/>
-    </row>
-    <row r="3" spans="1:19" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="T2" s="46"/>
+    </row>
+    <row r="3" spans="1:20" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C3" s="29" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="39" t="s">
+      <c r="E3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="35" t="s">
-        <v>160</v>
+      <c r="G3" s="30" t="s">
+        <v>9</v>
       </c>
       <c r="H3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="I3" s="35" t="s">
+        <v>159</v>
+      </c>
+      <c r="L3" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="L3" s="30" t="s">
-        <v>9</v>
-      </c>
       <c r="M3" s="30" t="s">
         <v>9</v>
       </c>
       <c r="N3" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="40" t="s">
+      <c r="O3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q3" s="29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q3" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C4" s="31" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="G4" s="32" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="35" t="s">
+      <c r="I4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="L4" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="M4" s="32" t="s">
         <v>9</v>
       </c>
       <c r="N4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="35" t="s">
+      <c r="O4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="P4" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q4" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="S4" s="31" t="s">
+      <c r="Q4" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R4" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="T4" s="31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C5" s="31" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="G5" s="32" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="I5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="L5" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="M5" s="32" t="s">
         <v>9</v>
       </c>
       <c r="N5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O5" s="39" t="s">
+      <c r="O5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q5" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="S5" s="31" t="s">
+      <c r="Q5" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R5" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="T5" s="31" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="31" t="s">
         <v>61</v>
       </c>
       <c r="D6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="H6" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K6" s="39" t="s">
+      <c r="I6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="39" t="s">
         <v>79</v>
-      </c>
-      <c r="L6" s="38" t="s">
-        <v>60</v>
       </c>
       <c r="M6" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O6" s="38" t="s">
+      <c r="N6" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P6" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q6" s="29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P6" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q6" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R6" s="29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C7" s="31" t="s">
         <v>77</v>
       </c>
       <c r="D7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="E7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="32" t="s">
         <v>9</v>
       </c>
       <c r="H7" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="L7" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="L7" s="36" t="s">
+      <c r="M7" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M7" s="38" t="s">
+      <c r="N7" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O7" s="38" t="s">
+      <c r="O7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P7" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q7" s="31" t="s">
+      <c r="Q7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R7" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="S7" s="33" t="s">
+      <c r="T7" s="33" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C8" s="31" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="G8" s="32" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="39" t="s">
+      <c r="I8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="L8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="38" t="s">
+      <c r="M8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N8" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O8" s="39" t="s">
+      <c r="O8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P8" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q8" s="31" t="s">
+      <c r="Q8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R8" s="31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C9" s="31" t="s">
         <v>150</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="E9" s="32" t="s">
         <v>9</v>
       </c>
       <c r="G9" s="32" t="s">
@@ -2006,660 +2104,684 @@
       <c r="H9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="35" t="s">
+      <c r="I9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="L9" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M9" s="38" t="s">
+      <c r="M9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N9" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P9" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="P9" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q9" s="31" t="s">
+      <c r="Q9" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R9" s="31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C10" s="31" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L10" s="36" t="s">
+      <c r="E10" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N10" s="38" t="s">
+      <c r="N10" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O10" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="O10" s="35" t="s">
+      <c r="P10" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="P10" s="38" t="s">
+      <c r="Q10" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q10" s="31" t="s">
+      <c r="R10" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="S10" s="31" t="s">
+      <c r="T10" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C13" s="31" t="s">
         <v>94</v>
       </c>
       <c r="D13" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="I13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L13" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="M13" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K13" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="L13" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="M13" s="38" t="s">
+      <c r="N13" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N13" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O13" s="38" t="s">
+      <c r="O13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P13" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P13" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q13" s="31" t="s">
+      <c r="Q13" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R13" s="31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="31" t="s">
         <v>3</v>
       </c>
       <c r="D14" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="G14" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="I14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M14" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L14" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="M14" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="N14" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O14" s="35" t="s">
+      <c r="O14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P14" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="P14" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q14" s="31" t="s">
+      <c r="Q14" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R14" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="S14" s="31" t="s">
+      <c r="T14" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C15" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="35" t="s">
-        <v>161</v>
-      </c>
-      <c r="K15" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L15" s="36" t="s">
+      <c r="I15" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="L15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M15" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M15" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="N15" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O15" s="35" t="s">
+      <c r="O15" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P15" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="P15" s="38" t="s">
+      <c r="Q15" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q15" s="31" t="s">
+      <c r="R15" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="S15" s="31" t="s">
+      <c r="T15" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C16" s="31" t="s">
         <v>82</v>
       </c>
       <c r="D16" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="I16" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="M16" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K16" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="L16" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="M16" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="N16" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O16" s="38" t="s">
+      <c r="O16" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P16" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P16" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q16" s="31" t="s">
+      <c r="Q16" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R16" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="S16" s="33" t="s">
+      <c r="T16" s="33" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C17" s="31" t="s">
         <v>95</v>
       </c>
       <c r="D17" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="I17" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L17" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M17" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K17" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L17" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="M17" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="N17" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O17" s="35" t="s">
+      <c r="O17" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P17" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="P17" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q17" s="31" t="s">
+      <c r="Q17" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R17" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="S17" s="31" t="s">
+      <c r="T17" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="31" t="s">
         <v>32</v>
       </c>
       <c r="H20" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K20" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L20" s="36" t="s">
+      <c r="L20" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M20" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N20" s="38" t="s">
+      <c r="N20" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O20" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="O20" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="P20" s="38" t="s">
+      <c r="P20" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q20" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q20" s="31" t="s">
+      <c r="R20" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="S20" s="31" t="s">
+      <c r="T20" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="31" t="s">
         <v>33</v>
       </c>
       <c r="H21" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L21" s="36" t="s">
+      <c r="L21" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="M21" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="M21" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N21" s="38" t="s">
+      <c r="N21" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O21" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="O21" s="35" t="s">
+      <c r="P21" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="P21" s="38" t="s">
+      <c r="Q21" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q21" s="31" t="s">
+      <c r="R21" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="S21" s="31" t="s">
+      <c r="T21" s="31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="35" t="s">
+      <c r="F24" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="F24" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K24" s="39" t="s">
+      <c r="G24" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L24" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="L24" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="M24" s="32" t="s">
         <v>9</v>
       </c>
       <c r="N24" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O24" s="35" t="s">
+      <c r="O24" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P24" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="P24" s="38" t="s">
+      <c r="Q24" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q24" s="31" t="s">
+      <c r="R24" s="31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="35" t="s">
+      <c r="F25" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="F25" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K25" s="35" t="s">
+      <c r="G25" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L25" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="L25" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M25" s="38" t="s">
+      <c r="M25" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N25" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N25" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O25" s="38" t="s">
-        <v>60</v>
+      <c r="O25" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="P25" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q25" s="31" t="s">
+      <c r="Q25" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="R25" s="31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="F26" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="F26" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K26" s="35" t="s">
+      <c r="G26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L26" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="L26" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="M26" s="32" t="s">
         <v>9</v>
       </c>
       <c r="N26" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O26" s="38" t="s">
+      <c r="O26" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P26" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P26" s="39" t="s">
+      <c r="Q26" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Q26" s="31" t="s">
+      <c r="R26" s="31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L27" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="M27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N27" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="O27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P27" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q27" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R27" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="D27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K27" s="35" t="s">
+      <c r="G28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L28" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="L27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M27" s="38" t="s">
+      <c r="M28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="O28" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P28" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q28" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O27" s="38" t="s">
+      <c r="R28" s="31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C29" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="39" t="s">
+        <v>161</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L29" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="M29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N29" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P27" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q27" s="31" t="s">
+      <c r="O29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P29" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q29" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="R29" s="31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K28" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="L28" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M28" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="N28" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O28" s="35" t="s">
-        <v>159</v>
-      </c>
-      <c r="P28" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q28" s="31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C29" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="D29" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="39" t="s">
-        <v>162</v>
-      </c>
-      <c r="F29" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K29" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="L29" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M29" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="N29" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O29" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="P29" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q29" s="31" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C32" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="39" t="s">
+      <c r="F32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K32" s="39" t="s">
+      <c r="J32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L32" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="L32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M32" s="38" t="s">
+      <c r="M32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N32" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O32" s="38" t="s">
+      <c r="O32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P32" s="39" t="s">
+      <c r="Q32" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Q32" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="S32" s="31" t="s">
+      <c r="R32" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="T32" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C33" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="39" t="s">
+      <c r="F33" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="I33" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K33" s="39" t="s">
+      <c r="J33" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L33" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="L33" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M33" s="38" t="s">
+      <c r="M33" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N33" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O33" s="38" t="s">
+      <c r="O33" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P33" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P33" s="39" t="s">
+      <c r="Q33" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Q33" s="29" t="s">
-        <v>155</v>
-      </c>
-      <c r="S33" s="31" t="s">
+      <c r="R33" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="T33" s="31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C34" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="F34" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="39" t="s">
+      <c r="G34" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="I34" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K34" s="39" t="s">
+      <c r="J34" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L34" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="L34" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="M34" s="32" t="s">
         <v>9</v>
       </c>
       <c r="N34" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O34" s="38" t="s">
+      <c r="O34" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="P34" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P34" s="39" t="s">
+      <c r="Q34" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="Q34" s="31" t="s">
+      <c r="R34" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="S34" s="31" t="s">
+      <c r="T34" s="31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="1:19" s="42" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
         <v>98</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="31" t="s">
         <v>92</v>
       </c>
@@ -2667,34 +2789,37 @@
         <v>23</v>
       </c>
       <c r="E37" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="39" t="s">
+      <c r="G37" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="K37" s="39" t="s">
+      <c r="L37" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="L37" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M37" s="38" t="s">
+      <c r="M37" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N37" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N37" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O37" s="38" t="s">
-        <v>60</v>
+      <c r="O37" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="P37" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q37" s="29" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="38" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Q37" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="R37" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="31" t="s">
         <v>93</v>
       </c>
@@ -2702,39 +2827,42 @@
         <v>23</v>
       </c>
       <c r="E38" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="F38" s="39" t="s">
+      <c r="G38" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="K38" s="35" t="s">
+      <c r="L38" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="L38" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="M38" s="38" t="s">
+      <c r="M38" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="N38" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N38" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="O38" s="38" t="s">
-        <v>60</v>
+      <c r="O38" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="P38" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q38" s="29" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q38" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="R38" s="29" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C39" s="41" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="47" t="s">
         <v>99</v>
       </c>
@@ -2742,458 +2870,498 @@
       <c r="C42" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="D42" s="51" t="s">
+      <c r="D42" s="50" t="s">
         <v>102</v>
       </c>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="K42" s="50" t="s">
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="50"/>
+      <c r="H42" s="50"/>
+      <c r="I42" s="50"/>
+      <c r="J42" s="50"/>
+      <c r="L42" s="49" t="s">
         <v>124</v>
       </c>
-      <c r="L42" s="50"/>
-      <c r="M42" s="50"/>
-      <c r="N42" s="50"/>
-      <c r="O42" s="50"/>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="50"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M42" s="49"/>
+      <c r="N42" s="49"/>
+      <c r="O42" s="49"/>
+      <c r="P42" s="49"/>
+      <c r="Q42" s="49"/>
+      <c r="R42" s="49"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>100</v>
       </c>
       <c r="C43" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="D43" s="48" t="s">
+      <c r="D43" s="54" t="s">
         <v>103</v>
       </c>
-      <c r="E43" s="48"/>
-      <c r="F43" s="48"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
-      <c r="K43" s="49" t="s">
+      <c r="E43" s="54"/>
+      <c r="F43" s="54"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="54"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
+      <c r="L43" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="L43" s="49"/>
-      <c r="M43" s="49"/>
-      <c r="N43" s="49"/>
-      <c r="O43" s="49"/>
-      <c r="P43" s="49"/>
-      <c r="Q43" s="49"/>
-      <c r="S43" s="53" t="s">
+      <c r="M43" s="48"/>
+      <c r="N43" s="48"/>
+      <c r="O43" s="48"/>
+      <c r="P43" s="48"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="48"/>
+      <c r="T43" s="52" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>114</v>
       </c>
       <c r="C44" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="D44" s="48" t="s">
+      <c r="D44" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="E44" s="48"/>
-      <c r="F44" s="48"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="K44" s="49" t="s">
+      <c r="E44" s="54"/>
+      <c r="F44" s="54"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="54"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="54"/>
+      <c r="L44" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="L44" s="49"/>
-      <c r="M44" s="49"/>
-      <c r="N44" s="49"/>
-      <c r="O44" s="49"/>
-      <c r="P44" s="49"/>
-      <c r="Q44" s="49"/>
-      <c r="S44" s="53" t="s">
+      <c r="M44" s="48"/>
+      <c r="N44" s="48"/>
+      <c r="O44" s="48"/>
+      <c r="P44" s="48"/>
+      <c r="Q44" s="48"/>
+      <c r="R44" s="48"/>
+      <c r="T44" s="52" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>115</v>
       </c>
       <c r="C45" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="D45" s="48" t="s">
+      <c r="D45" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="48"/>
-      <c r="H45" s="48"/>
-      <c r="I45" s="48"/>
-      <c r="K45" s="49" t="s">
+      <c r="E45" s="54"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="54"/>
+      <c r="L45" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="L45" s="49"/>
-      <c r="M45" s="49"/>
-      <c r="N45" s="49"/>
-      <c r="O45" s="49"/>
-      <c r="P45" s="49"/>
-      <c r="Q45" s="49"/>
-      <c r="S45" s="53" t="s">
+      <c r="M45" s="48"/>
+      <c r="N45" s="48"/>
+      <c r="O45" s="48"/>
+      <c r="P45" s="48"/>
+      <c r="Q45" s="48"/>
+      <c r="R45" s="48"/>
+      <c r="T45" s="52" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>116</v>
       </c>
       <c r="C46" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="48" t="s">
+      <c r="D46" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="48"/>
-      <c r="H46" s="48"/>
-      <c r="I46" s="48"/>
-      <c r="K46" s="49" t="s">
+      <c r="E46" s="54"/>
+      <c r="F46" s="54"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="54"/>
+      <c r="I46" s="54"/>
+      <c r="J46" s="54"/>
+      <c r="L46" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="L46" s="49"/>
-      <c r="M46" s="49"/>
-      <c r="N46" s="49"/>
-      <c r="O46" s="49"/>
-      <c r="P46" s="49"/>
-      <c r="Q46" s="49"/>
-      <c r="S46" s="53" t="s">
+      <c r="M46" s="48"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="48"/>
+      <c r="P46" s="48"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="48"/>
+      <c r="T46" s="52" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>117</v>
       </c>
       <c r="C47" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="48" t="s">
+      <c r="D47" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="48"/>
-      <c r="H47" s="48"/>
-      <c r="I47" s="48"/>
-      <c r="K47" s="49" t="s">
+      <c r="E47" s="54"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="54"/>
+      <c r="L47" s="48" t="s">
         <v>136</v>
       </c>
-      <c r="L47" s="49"/>
-      <c r="M47" s="49"/>
-      <c r="N47" s="49"/>
-      <c r="O47" s="49"/>
-      <c r="P47" s="49"/>
-      <c r="Q47" s="49"/>
-      <c r="S47" s="53" t="s">
+      <c r="M47" s="48"/>
+      <c r="N47" s="48"/>
+      <c r="O47" s="48"/>
+      <c r="P47" s="48"/>
+      <c r="Q47" s="48"/>
+      <c r="R47" s="48"/>
+      <c r="T47" s="52" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>118</v>
       </c>
       <c r="C48" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="D48" s="48" t="s">
+      <c r="D48" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="48"/>
-      <c r="H48" s="48"/>
-      <c r="I48" s="48"/>
-      <c r="K48" s="49" t="s">
+      <c r="E48" s="54"/>
+      <c r="F48" s="54"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="54"/>
+      <c r="J48" s="54"/>
+      <c r="L48" s="48" t="s">
         <v>135</v>
       </c>
-      <c r="L48" s="49"/>
-      <c r="M48" s="49"/>
-      <c r="N48" s="49"/>
-      <c r="O48" s="49"/>
-      <c r="P48" s="49"/>
-      <c r="Q48" s="49"/>
-      <c r="S48" s="53" t="s">
+      <c r="M48" s="48"/>
+      <c r="N48" s="48"/>
+      <c r="O48" s="48"/>
+      <c r="P48" s="48"/>
+      <c r="Q48" s="48"/>
+      <c r="R48" s="48"/>
+      <c r="T48" s="52" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>119</v>
       </c>
       <c r="C49" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="D49" s="48" t="s">
+      <c r="D49" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-      <c r="I49" s="48"/>
-      <c r="K49" s="49" t="s">
+      <c r="E49" s="54"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="54"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="54"/>
+      <c r="L49" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="L49" s="49"/>
-      <c r="M49" s="49"/>
-      <c r="N49" s="49"/>
-      <c r="O49" s="49"/>
-      <c r="P49" s="49"/>
-      <c r="Q49" s="49"/>
-      <c r="S49" s="53" t="s">
+      <c r="M49" s="48"/>
+      <c r="N49" s="48"/>
+      <c r="O49" s="48"/>
+      <c r="P49" s="48"/>
+      <c r="Q49" s="48"/>
+      <c r="R49" s="48"/>
+      <c r="T49" s="52" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>120</v>
       </c>
       <c r="C50" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="D50" s="48" t="s">
+      <c r="D50" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="48"/>
-      <c r="K50" s="49" t="s">
+      <c r="E50" s="54"/>
+      <c r="F50" s="54"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="54"/>
+      <c r="L50" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="L50" s="49"/>
-      <c r="M50" s="49"/>
-      <c r="N50" s="49"/>
-      <c r="O50" s="49"/>
-      <c r="P50" s="49"/>
-      <c r="Q50" s="49"/>
-      <c r="S50" s="28" t="s">
+      <c r="M50" s="48"/>
+      <c r="N50" s="48"/>
+      <c r="O50" s="48"/>
+      <c r="P50" s="48"/>
+      <c r="Q50" s="48"/>
+      <c r="R50" s="48"/>
+      <c r="T50" s="28" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>121</v>
       </c>
       <c r="C51" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="D51" s="48" t="s">
+      <c r="D51" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="48"/>
-      <c r="K51" s="49" t="s">
+      <c r="E51" s="54"/>
+      <c r="F51" s="54"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="54"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="54"/>
+      <c r="L51" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="L51" s="49"/>
-      <c r="M51" s="49"/>
-      <c r="N51" s="49"/>
-      <c r="O51" s="49"/>
-      <c r="P51" s="49"/>
-      <c r="Q51" s="49"/>
-      <c r="S51" s="28" t="s">
+      <c r="M51" s="48"/>
+      <c r="N51" s="48"/>
+      <c r="O51" s="48"/>
+      <c r="P51" s="48"/>
+      <c r="Q51" s="48"/>
+      <c r="R51" s="48"/>
+      <c r="T51" s="28" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>122</v>
       </c>
       <c r="C52" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="D52" s="48" t="s">
+      <c r="D52" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="E52" s="48"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="48"/>
-      <c r="H52" s="48"/>
-      <c r="I52" s="48"/>
-      <c r="K52" s="49" t="s">
+      <c r="E52" s="54"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="54"/>
+      <c r="H52" s="54"/>
+      <c r="I52" s="54"/>
+      <c r="J52" s="54"/>
+      <c r="L52" s="48" t="s">
         <v>126</v>
       </c>
-      <c r="L52" s="49"/>
-      <c r="M52" s="49"/>
-      <c r="N52" s="49"/>
-      <c r="O52" s="49"/>
-      <c r="P52" s="49"/>
-      <c r="Q52" s="49"/>
-      <c r="S52" s="28" t="s">
+      <c r="M52" s="48"/>
+      <c r="N52" s="48"/>
+      <c r="O52" s="48"/>
+      <c r="P52" s="48"/>
+      <c r="Q52" s="48"/>
+      <c r="R52" s="48"/>
+      <c r="T52" s="28" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>123</v>
       </c>
       <c r="C53" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="D53" s="48" t="s">
+      <c r="D53" s="54" t="s">
         <v>113</v>
       </c>
-      <c r="E53" s="48"/>
-      <c r="F53" s="48"/>
-      <c r="G53" s="48"/>
-      <c r="H53" s="48"/>
-      <c r="I53" s="48"/>
-      <c r="K53" s="49" t="s">
+      <c r="E53" s="54"/>
+      <c r="F53" s="54"/>
+      <c r="G53" s="54"/>
+      <c r="H53" s="54"/>
+      <c r="I53" s="54"/>
+      <c r="J53" s="54"/>
+      <c r="L53" s="48" t="s">
         <v>125</v>
       </c>
-      <c r="L53" s="49"/>
-      <c r="M53" s="49"/>
-      <c r="N53" s="49"/>
-      <c r="O53" s="49"/>
-      <c r="P53" s="49"/>
-      <c r="Q53" s="49"/>
-      <c r="S53" s="34" t="s">
+      <c r="M53" s="48"/>
+      <c r="N53" s="48"/>
+      <c r="O53" s="48"/>
+      <c r="P53" s="48"/>
+      <c r="Q53" s="48"/>
+      <c r="R53" s="48"/>
+      <c r="T53" s="34" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="63" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C63" s="31" t="s">
         <v>57</v>
       </c>
       <c r="D63" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="E63" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="F63" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G63" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="H63" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="K63" s="37" t="s">
+      <c r="L63" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="L63" s="32" t="s">
-        <v>9</v>
-      </c>
       <c r="M63" s="32" t="s">
         <v>9</v>
       </c>
       <c r="N63" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="O63" s="30"/>
+      <c r="O63" s="32" t="s">
+        <v>9</v>
+      </c>
       <c r="P63" s="30"/>
       <c r="Q63" s="30"/>
+      <c r="R63" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="D52:I52"/>
-    <mergeCell ref="D53:I53"/>
-    <mergeCell ref="D42:I42"/>
-    <mergeCell ref="D43:I43"/>
-    <mergeCell ref="D44:I44"/>
-    <mergeCell ref="D45:I45"/>
-    <mergeCell ref="K52:Q52"/>
-    <mergeCell ref="K53:Q53"/>
-    <mergeCell ref="K42:Q42"/>
-    <mergeCell ref="K43:Q43"/>
-    <mergeCell ref="K44:Q44"/>
-    <mergeCell ref="K45:Q45"/>
-    <mergeCell ref="K46:Q46"/>
-    <mergeCell ref="K47:Q47"/>
-    <mergeCell ref="D51:I51"/>
-    <mergeCell ref="K48:Q48"/>
-    <mergeCell ref="K49:Q49"/>
-    <mergeCell ref="K50:Q50"/>
-    <mergeCell ref="K51:Q51"/>
-    <mergeCell ref="D46:I46"/>
-    <mergeCell ref="D47:I47"/>
-    <mergeCell ref="D48:I48"/>
-    <mergeCell ref="D49:I49"/>
-    <mergeCell ref="D50:I50"/>
+    <mergeCell ref="D52:J52"/>
+    <mergeCell ref="D53:J53"/>
+    <mergeCell ref="D42:J42"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="D44:J44"/>
+    <mergeCell ref="D45:J45"/>
+    <mergeCell ref="D46:J46"/>
+    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="D48:J48"/>
+    <mergeCell ref="D49:J49"/>
+    <mergeCell ref="D50:J50"/>
+    <mergeCell ref="D51:J51"/>
+    <mergeCell ref="L52:R52"/>
+    <mergeCell ref="L53:R53"/>
+    <mergeCell ref="L42:R42"/>
+    <mergeCell ref="L43:R43"/>
+    <mergeCell ref="L44:R44"/>
+    <mergeCell ref="L45:R45"/>
+    <mergeCell ref="L46:R46"/>
+    <mergeCell ref="L47:R47"/>
+    <mergeCell ref="L48:R48"/>
+    <mergeCell ref="L49:R49"/>
+    <mergeCell ref="L50:R50"/>
+    <mergeCell ref="L51:R51"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="D63 D18 D16 D14 D24:D26 D32:D35 D30 D20:D22 D3:D11">
-    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
+  <conditionalFormatting sqref="E18 E14 E24:E26 E32:E35 E30 E20:E22 E3:E11 J13:K13 H13">
+    <cfRule type="cellIs" dxfId="20" priority="29" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D19">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:G14">
+    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63 D18 D14 D24:D26 D32:D35 D30 D20:D22 D3:D11">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="9" priority="13" operator="equal">
-      <formula>"ja"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="equal">
-      <formula>"ja"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13:J13">
     <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D31">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>"ja"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+  <conditionalFormatting sqref="D13">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
+  <conditionalFormatting sqref="D28">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
+  <conditionalFormatting sqref="D16:G17">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="S43" r:id="rId1" xr:uid="{2F2AC83B-E3C5-42BC-A8AB-1C13D82BD690}"/>
-    <hyperlink ref="S44" r:id="rId2" xr:uid="{0FBD89B3-32F8-40AC-842E-8AD0D2B6C2F3}"/>
-    <hyperlink ref="S45" r:id="rId3" xr:uid="{620B8347-8EF9-46A1-BCD7-CC9AC99A521B}"/>
-    <hyperlink ref="S46" r:id="rId4" xr:uid="{52BB097F-4337-40BC-8429-4EAACC609E96}"/>
-    <hyperlink ref="S47" r:id="rId5" xr:uid="{86D7D8D2-4A6F-429E-82A4-8F3837AB5B83}"/>
-    <hyperlink ref="S48" r:id="rId6" xr:uid="{04E81D6C-FFE2-491C-ADE3-C5A4302B59D8}"/>
-    <hyperlink ref="S49" r:id="rId7" xr:uid="{01914F05-ABA5-4B96-8522-4554F7DCD64D}"/>
+    <hyperlink ref="T43" r:id="rId1" xr:uid="{2F2AC83B-E3C5-42BC-A8AB-1C13D82BD690}"/>
+    <hyperlink ref="T44" r:id="rId2" xr:uid="{0FBD89B3-32F8-40AC-842E-8AD0D2B6C2F3}"/>
+    <hyperlink ref="T45" r:id="rId3" xr:uid="{620B8347-8EF9-46A1-BCD7-CC9AC99A521B}"/>
+    <hyperlink ref="T46" r:id="rId4" xr:uid="{52BB097F-4337-40BC-8429-4EAACC609E96}"/>
+    <hyperlink ref="T47" r:id="rId5" xr:uid="{86D7D8D2-4A6F-429E-82A4-8F3837AB5B83}"/>
+    <hyperlink ref="T48" r:id="rId6" xr:uid="{04E81D6C-FFE2-491C-ADE3-C5A4302B59D8}"/>
+    <hyperlink ref="T49" r:id="rId7" xr:uid="{01914F05-ABA5-4B96-8522-4554F7DCD64D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
@@ -3426,15 +3594,15 @@
       <c r="B9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="52" t="s">
+      <c r="C9" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="52"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
       <c r="J9" s="3" t="s">
         <v>19</v>
       </c>
@@ -3520,15 +3688,15 @@
       <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="52"/>
-      <c r="G13" s="52"/>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="51"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="51"/>
       <c r="J13" s="3" t="s">
         <v>19</v>
       </c>
@@ -3541,15 +3709,15 @@
       <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
       <c r="J14" s="3" t="s">
         <v>19</v>
       </c>
@@ -3606,15 +3774,15 @@
       <c r="B17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-      <c r="I17" s="52"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
       <c r="J17" s="3" t="s">
         <v>19</v>
       </c>
@@ -3627,15 +3795,15 @@
       <c r="B18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="52"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="52"/>
+      <c r="D18" s="51"/>
+      <c r="E18" s="51"/>
+      <c r="F18" s="51"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
       <c r="J18" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
[ELAB-414] rework of 'Werkzeuge und Technologien'^8
</commit_message>
<xml_diff>
--- a/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
+++ b/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\tools-und-werkzeuge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB94005-2355-4F22-A5B5-B0F55042542A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05A5FCD-A2EC-447F-8801-A55D6D72C7BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="alte Ansicht" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -314,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="164">
   <si>
     <t>Sentry</t>
   </si>
@@ -545,9 +544,6 @@
  - Cloud Lösung auf 60 Tage begrenzt, OnPremise unbegrenzt</t>
   </si>
   <si>
-    <t>gruppiert</t>
-  </si>
-  <si>
     <t>Technologie</t>
   </si>
   <si>
@@ -569,9 +565,6 @@
     <t>TABLE_END</t>
   </si>
   <si>
-    <t>bei \mbox{Fehlern}</t>
-  </si>
-  <si>
     <t>Splunk \mbox{Enterprise}</t>
   </si>
   <si>
@@ -590,18 +583,12 @@
     <t>Zielgruppe</t>
   </si>
   <si>
-    <t>geringfügig</t>
-  </si>
-  <si>
     <t>Fachabteilung, Entwickler</t>
   </si>
   <si>
     <t>Entwickler</t>
   </si>
   <si>
-    <t>nein, aber quelloffen</t>
-  </si>
-  <si>
     <t>Google Analytics</t>
   </si>
   <si>
@@ -800,18 +787,6 @@
     <t>Ignore</t>
   </si>
   <si>
-    <t>nein, aber teils quelloffen</t>
-  </si>
-  <si>
-    <t>mit Erw.</t>
-  </si>
-  <si>
-    <t>nur Agg.</t>
-  </si>
-  <si>
-    <t>grupp. und bei \mbox{Fehlern}</t>
-  </si>
-  <si>
     <t>Log-Plattform</t>
   </si>
   <si>
@@ -827,13 +802,19 @@
     <t>IM</t>
   </si>
   <si>
-    <t>mögl.</t>
-  </si>
-  <si>
     <t>APM-Plattform</t>
   </si>
   <si>
     <t>Session-Replay-Dienst</t>
+  </si>
+  <si>
+    <t>eingeschr.</t>
+  </si>
+  <si>
+    <t>ja(*)</t>
+  </si>
+  <si>
+    <t>eing.</t>
   </si>
 </sst>
 </file>
@@ -1219,22 +1200,22 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1246,7 +1227,63 @@
     <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="29">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1712,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FA36FA-A460-4BBC-B832-96B5FC35BB7A}">
   <dimension ref="A1:T63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F3:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,7 +1761,7 @@
     <col min="4" max="4" width="8.7109375" style="28" customWidth="1"/>
     <col min="5" max="5" width="8.140625" style="28" customWidth="1"/>
     <col min="6" max="6" width="11.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="28" customWidth="1"/>
     <col min="8" max="8" width="8.140625" style="28" customWidth="1"/>
     <col min="9" max="9" width="14.140625" style="28" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" style="28" customWidth="1"/>
@@ -1742,31 +1779,31 @@
   <sheetData>
     <row r="1" spans="1:20" s="43" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>96</v>
-      </c>
-      <c r="B1" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="49" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="44" t="s">
         <v>157</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="D1" s="44" t="s">
-        <v>166</v>
-      </c>
-      <c r="E1" s="44" t="s">
-        <v>165</v>
       </c>
       <c r="F1" s="44" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H1" s="44" t="s">
         <v>34</v>
       </c>
       <c r="I1" s="44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J1" s="44" t="s">
         <v>66</v>
@@ -1776,22 +1813,22 @@
         <v>58</v>
       </c>
       <c r="M1" s="44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N1" s="44" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="O1" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q1" s="44" t="s">
+        <v>82</v>
+      </c>
+      <c r="R1" s="44" t="s">
         <v>85</v>
-      </c>
-      <c r="P1" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q1" s="44" t="s">
-        <v>84</v>
-      </c>
-      <c r="R1" s="44" t="s">
-        <v>87</v>
       </c>
       <c r="S1" s="44"/>
       <c r="T1" s="44" t="s">
@@ -1800,10 +1837,10 @@
     </row>
     <row r="2" spans="1:20" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
@@ -1835,7 +1872,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>9</v>
@@ -1844,10 +1881,10 @@
         <v>9</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L3" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M3" s="30" t="s">
         <v>9</v>
@@ -1859,13 +1896,13 @@
         <v>9</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>23</v>
+        <v>161</v>
       </c>
       <c r="Q3" s="30" t="s">
         <v>9</v>
       </c>
       <c r="R3" s="29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -1879,7 +1916,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="G4" s="32" t="s">
         <v>9</v>
@@ -1891,7 +1928,7 @@
         <v>9</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M4" s="32" t="s">
         <v>9</v>
@@ -1902,14 +1939,14 @@
       <c r="O4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="35" t="s">
-        <v>88</v>
+      <c r="P4" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q4" s="32" t="s">
         <v>9</v>
       </c>
       <c r="R4" s="29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="T4" s="31" t="s">
         <v>62</v>
@@ -1926,7 +1963,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="G5" s="32" t="s">
         <v>9</v>
@@ -1938,7 +1975,7 @@
         <v>9</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M5" s="32" t="s">
         <v>9</v>
@@ -1949,14 +1986,14 @@
       <c r="O5" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P5" s="39" t="s">
-        <v>23</v>
+      <c r="P5" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q5" s="32" t="s">
         <v>9</v>
       </c>
       <c r="R5" s="29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="T5" s="31" t="s">
         <v>63</v>
@@ -1982,7 +2019,7 @@
         <v>9</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M6" s="38" t="s">
         <v>60</v>
@@ -2000,30 +2037,30 @@
         <v>9</v>
       </c>
       <c r="R6" s="29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C7" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="L7" s="35" t="s">
-        <v>78</v>
-      </c>
       <c r="M7" s="36" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="N7" s="38" t="s">
         <v>60</v>
@@ -2038,7 +2075,7 @@
         <v>9</v>
       </c>
       <c r="R7" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T7" s="33" t="s">
         <v>56</v>
@@ -2055,7 +2092,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="G8" s="32" t="s">
         <v>9</v>
@@ -2067,7 +2104,7 @@
         <v>9</v>
       </c>
       <c r="L8" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M8" s="32" t="s">
         <v>9</v>
@@ -2078,19 +2115,19 @@
       <c r="O8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P8" s="39" t="s">
-        <v>23</v>
+      <c r="P8" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q8" s="32" t="s">
         <v>9</v>
       </c>
       <c r="R8" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C9" s="31" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D9" s="32" t="s">
         <v>9</v>
@@ -2108,7 +2145,7 @@
         <v>9</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M9" s="32" t="s">
         <v>9</v>
@@ -2119,14 +2156,14 @@
       <c r="O9" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P9" s="39" t="s">
-        <v>23</v>
+      <c r="P9" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q9" s="32" t="s">
         <v>9</v>
       </c>
       <c r="R9" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2143,7 +2180,7 @@
         <v>9</v>
       </c>
       <c r="M10" s="36" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="N10" s="32" t="s">
         <v>9</v>
@@ -2151,14 +2188,14 @@
       <c r="O10" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P10" s="35" t="s">
-        <v>91</v>
+      <c r="P10" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q10" s="38" t="s">
         <v>60</v>
       </c>
       <c r="R10" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T10" s="31" t="s">
         <v>35</v>
@@ -2167,33 +2204,33 @@
     <row r="11" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C13" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="F13" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="G13" s="36" t="s">
-        <v>167</v>
+        <v>90</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="G13" s="39" t="s">
+        <v>162</v>
       </c>
       <c r="I13" s="32" t="s">
         <v>9</v>
       </c>
       <c r="L13" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M13" s="36" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="N13" s="38" t="s">
         <v>60</v>
@@ -2208,24 +2245,24 @@
         <v>9</v>
       </c>
       <c r="R13" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>167</v>
+      <c r="D14" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>162</v>
       </c>
       <c r="I14" s="32" t="s">
         <v>9</v>
@@ -2234,7 +2271,7 @@
         <v>9</v>
       </c>
       <c r="M14" s="36" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="N14" s="32" t="s">
         <v>9</v>
@@ -2242,14 +2279,14 @@
       <c r="O14" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P14" s="35" t="s">
-        <v>91</v>
+      <c r="P14" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q14" s="32" t="s">
         <v>9</v>
       </c>
       <c r="R14" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T14" s="31" t="s">
         <v>35</v>
@@ -2260,13 +2297,13 @@
         <v>71</v>
       </c>
       <c r="I15" s="35" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L15" s="32" t="s">
         <v>9</v>
       </c>
       <c r="M15" s="36" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="N15" s="32" t="s">
         <v>9</v>
@@ -2274,14 +2311,14 @@
       <c r="O15" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P15" s="35" t="s">
-        <v>91</v>
+      <c r="P15" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q15" s="38" t="s">
         <v>60</v>
       </c>
       <c r="R15" s="31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T15" s="31" t="s">
         <v>35</v>
@@ -2289,28 +2326,28 @@
     </row>
     <row r="16" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C16" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>167</v>
+        <v>80</v>
+      </c>
+      <c r="D16" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="F16" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="G16" s="39" t="s">
+        <v>162</v>
       </c>
       <c r="I16" s="32" t="s">
         <v>9</v>
       </c>
       <c r="L16" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M16" s="36" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="N16" s="32" t="s">
         <v>9</v>
@@ -2325,7 +2362,7 @@
         <v>9</v>
       </c>
       <c r="R16" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T16" s="33" t="s">
         <v>72</v>
@@ -2333,19 +2370,19 @@
     </row>
     <row r="17" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C17" s="31" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="F17" s="36" t="s">
-        <v>167</v>
-      </c>
-      <c r="G17" s="36" t="s">
-        <v>167</v>
+        <v>91</v>
+      </c>
+      <c r="D17" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="F17" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="G17" s="39" t="s">
+        <v>162</v>
       </c>
       <c r="I17" s="32" t="s">
         <v>9</v>
@@ -2354,7 +2391,7 @@
         <v>9</v>
       </c>
       <c r="M17" s="36" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="N17" s="32" t="s">
         <v>9</v>
@@ -2362,14 +2399,14 @@
       <c r="O17" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P17" s="35" t="s">
-        <v>91</v>
+      <c r="P17" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q17" s="32" t="s">
         <v>9</v>
       </c>
       <c r="R17" s="31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T17" s="31" t="s">
         <v>35</v>
@@ -2378,7 +2415,7 @@
     <row r="18" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2392,7 +2429,7 @@
         <v>9</v>
       </c>
       <c r="M20" s="36" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="N20" s="32" t="s">
         <v>9</v>
@@ -2407,7 +2444,7 @@
         <v>60</v>
       </c>
       <c r="R20" s="31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T20" s="31" t="s">
         <v>35</v>
@@ -2424,7 +2461,7 @@
         <v>9</v>
       </c>
       <c r="M21" s="36" t="s">
-        <v>16</v>
+        <v>161</v>
       </c>
       <c r="N21" s="32" t="s">
         <v>9</v>
@@ -2432,14 +2469,14 @@
       <c r="O21" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="P21" s="35" t="s">
-        <v>91</v>
+      <c r="P21" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q21" s="38" t="s">
         <v>60</v>
       </c>
       <c r="R21" s="31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T21" s="31" t="s">
         <v>35</v>
@@ -2448,21 +2485,21 @@
     <row r="22" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C24" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="F24" s="35" t="s">
-        <v>81</v>
+      <c r="F24" s="39" t="s">
+        <v>162</v>
       </c>
       <c r="G24" s="32" t="s">
         <v>9</v>
       </c>
       <c r="L24" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M24" s="32" t="s">
         <v>9</v>
@@ -2473,28 +2510,28 @@
       <c r="O24" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P24" s="35" t="s">
-        <v>91</v>
+      <c r="P24" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q24" s="38" t="s">
         <v>60</v>
       </c>
       <c r="R24" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C25" s="31" t="s">
         <v>64</v>
       </c>
-      <c r="F25" s="35" t="s">
-        <v>81</v>
+      <c r="F25" s="39" t="s">
+        <v>162</v>
       </c>
       <c r="G25" s="32" t="s">
         <v>9</v>
       </c>
       <c r="L25" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M25" s="32" t="s">
         <v>9</v>
@@ -2512,21 +2549,21 @@
         <v>60</v>
       </c>
       <c r="R25" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C26" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="35" t="s">
-        <v>81</v>
+      <c r="F26" s="39" t="s">
+        <v>162</v>
       </c>
       <c r="G26" s="32" t="s">
         <v>9</v>
       </c>
       <c r="L26" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M26" s="32" t="s">
         <v>9</v>
@@ -2540,16 +2577,16 @@
       <c r="P26" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q26" s="39" t="s">
-        <v>23</v>
+      <c r="Q26" s="38" t="s">
+        <v>60</v>
       </c>
       <c r="R26" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C27" s="31" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D27" s="32" t="s">
         <v>9</v>
@@ -2561,7 +2598,7 @@
         <v>9</v>
       </c>
       <c r="L27" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M27" s="32" t="s">
         <v>9</v>
@@ -2579,18 +2616,18 @@
         <v>9</v>
       </c>
       <c r="R27" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C28" s="31" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G28" s="32" t="s">
         <v>9</v>
       </c>
       <c r="L28" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M28" s="32" t="s">
         <v>9</v>
@@ -2601,19 +2638,19 @@
       <c r="O28" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="P28" s="35" t="s">
-        <v>158</v>
+      <c r="P28" s="40" t="s">
+        <v>161</v>
       </c>
       <c r="Q28" s="38" t="s">
         <v>60</v>
       </c>
       <c r="R28" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C29" s="31" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D29" s="32" t="s">
         <v>9</v>
@@ -2622,13 +2659,13 @@
         <v>9</v>
       </c>
       <c r="F29" s="39" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G29" s="32" t="s">
         <v>9</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M29" s="32" t="s">
         <v>9</v>
@@ -2646,13 +2683,13 @@
         <v>9</v>
       </c>
       <c r="R29" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2669,7 +2706,7 @@
         <v>9</v>
       </c>
       <c r="L32" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M32" s="32" t="s">
         <v>9</v>
@@ -2683,11 +2720,11 @@
       <c r="P32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q32" s="39" t="s">
-        <v>23</v>
+      <c r="Q32" s="38" t="s">
+        <v>60</v>
       </c>
       <c r="R32" s="29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="T32" s="31" t="s">
         <v>70</v>
@@ -2707,7 +2744,7 @@
         <v>9</v>
       </c>
       <c r="L33" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M33" s="32" t="s">
         <v>9</v>
@@ -2721,11 +2758,11 @@
       <c r="P33" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q33" s="39" t="s">
-        <v>23</v>
+      <c r="Q33" s="38" t="s">
+        <v>60</v>
       </c>
       <c r="R33" s="29" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="T33" s="31" t="s">
         <v>68</v>
@@ -2741,14 +2778,11 @@
       <c r="G34" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="I34" s="39" t="s">
-        <v>23</v>
-      </c>
       <c r="J34" s="32" t="s">
         <v>9</v>
       </c>
       <c r="L34" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M34" s="32" t="s">
         <v>9</v>
@@ -2762,11 +2796,11 @@
       <c r="P34" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q34" s="39" t="s">
-        <v>23</v>
+      <c r="Q34" s="38" t="s">
+        <v>60</v>
       </c>
       <c r="R34" s="31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T34" s="31" t="s">
         <v>70</v>
@@ -2775,30 +2809,30 @@
     <row r="35" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="42" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="37" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C37" s="31" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>23</v>
+        <v>163</v>
       </c>
       <c r="E37" s="39" t="s">
-        <v>23</v>
+        <v>163</v>
       </c>
       <c r="F37" s="39" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="G37" s="39" t="s">
-        <v>23</v>
+        <v>161</v>
       </c>
       <c r="L37" s="39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M37" s="32" t="s">
         <v>9</v>
@@ -2816,27 +2850,27 @@
         <v>60</v>
       </c>
       <c r="R37" s="29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="38" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C38" s="31" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>23</v>
+        <v>163</v>
       </c>
       <c r="E38" s="39" t="s">
-        <v>23</v>
+        <v>163</v>
       </c>
       <c r="F38" s="39" t="s">
-        <v>73</v>
+        <v>162</v>
       </c>
       <c r="G38" s="39" t="s">
-        <v>23</v>
+        <v>161</v>
       </c>
       <c r="L38" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M38" s="32" t="s">
         <v>9</v>
@@ -2854,358 +2888,358 @@
         <v>60</v>
       </c>
       <c r="R38" s="29" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C39" s="41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="47" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B42" s="47"/>
       <c r="C42" s="47" t="s">
-        <v>130</v>
-      </c>
-      <c r="D42" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="E42" s="50"/>
-      <c r="F42" s="50"/>
-      <c r="G42" s="50"/>
-      <c r="H42" s="50"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="50"/>
-      <c r="L42" s="49" t="s">
-        <v>124</v>
-      </c>
-      <c r="M42" s="49"/>
-      <c r="N42" s="49"/>
-      <c r="O42" s="49"/>
-      <c r="P42" s="49"/>
-      <c r="Q42" s="49"/>
-      <c r="R42" s="49"/>
+        <v>126</v>
+      </c>
+      <c r="D42" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
+      <c r="L42" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="M42" s="53"/>
+      <c r="N42" s="53"/>
+      <c r="O42" s="53"/>
+      <c r="P42" s="53"/>
+      <c r="Q42" s="53"/>
+      <c r="R42" s="53"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C43" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="D43" s="54" t="s">
-        <v>103</v>
-      </c>
-      <c r="E43" s="54"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
-      <c r="L43" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="M43" s="48"/>
-      <c r="N43" s="48"/>
-      <c r="O43" s="48"/>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
-      <c r="R43" s="48"/>
-      <c r="T43" s="52" t="s">
-        <v>138</v>
+        <v>127</v>
+      </c>
+      <c r="D43" s="50" t="s">
+        <v>99</v>
+      </c>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
+      <c r="L43" s="52" t="s">
+        <v>97</v>
+      </c>
+      <c r="M43" s="52"/>
+      <c r="N43" s="52"/>
+      <c r="O43" s="52"/>
+      <c r="P43" s="52"/>
+      <c r="Q43" s="52"/>
+      <c r="R43" s="52"/>
+      <c r="T43" s="48" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C44" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="54" t="s">
-        <v>104</v>
-      </c>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="54"/>
-      <c r="J44" s="54"/>
-      <c r="L44" s="48" t="s">
-        <v>149</v>
-      </c>
-      <c r="M44" s="48"/>
-      <c r="N44" s="48"/>
-      <c r="O44" s="48"/>
-      <c r="P44" s="48"/>
-      <c r="Q44" s="48"/>
-      <c r="R44" s="48"/>
-      <c r="T44" s="52" t="s">
-        <v>139</v>
+        <v>128</v>
+      </c>
+      <c r="D44" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="I44" s="50"/>
+      <c r="J44" s="50"/>
+      <c r="L44" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="M44" s="52"/>
+      <c r="N44" s="52"/>
+      <c r="O44" s="52"/>
+      <c r="P44" s="52"/>
+      <c r="Q44" s="52"/>
+      <c r="R44" s="52"/>
+      <c r="T44" s="48" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C45" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="D45" s="54" t="s">
-        <v>105</v>
-      </c>
-      <c r="E45" s="54"/>
-      <c r="F45" s="54"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="54"/>
-      <c r="I45" s="54"/>
-      <c r="J45" s="54"/>
-      <c r="L45" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="M45" s="48"/>
-      <c r="N45" s="48"/>
-      <c r="O45" s="48"/>
-      <c r="P45" s="48"/>
-      <c r="Q45" s="48"/>
-      <c r="R45" s="48"/>
-      <c r="T45" s="52" t="s">
-        <v>140</v>
+        <v>128</v>
+      </c>
+      <c r="D45" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="50"/>
+      <c r="J45" s="50"/>
+      <c r="L45" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="M45" s="52"/>
+      <c r="N45" s="52"/>
+      <c r="O45" s="52"/>
+      <c r="P45" s="52"/>
+      <c r="Q45" s="52"/>
+      <c r="R45" s="52"/>
+      <c r="T45" s="48" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="D46" s="54" t="s">
-        <v>106</v>
-      </c>
-      <c r="E46" s="54"/>
-      <c r="F46" s="54"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="54"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="54"/>
-      <c r="L46" s="48" t="s">
-        <v>129</v>
-      </c>
-      <c r="M46" s="48"/>
-      <c r="N46" s="48"/>
-      <c r="O46" s="48"/>
-      <c r="P46" s="48"/>
-      <c r="Q46" s="48"/>
-      <c r="R46" s="48"/>
-      <c r="T46" s="52" t="s">
-        <v>141</v>
+        <v>128</v>
+      </c>
+      <c r="D46" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
+      <c r="L46" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="M46" s="52"/>
+      <c r="N46" s="52"/>
+      <c r="O46" s="52"/>
+      <c r="P46" s="52"/>
+      <c r="Q46" s="52"/>
+      <c r="R46" s="52"/>
+      <c r="T46" s="48" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C47" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D47" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="I47" s="50"/>
+      <c r="J47" s="50"/>
+      <c r="L47" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="54" t="s">
-        <v>107</v>
-      </c>
-      <c r="E47" s="54"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="54"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="54"/>
-      <c r="L47" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="M47" s="48"/>
-      <c r="N47" s="48"/>
-      <c r="O47" s="48"/>
-      <c r="P47" s="48"/>
-      <c r="Q47" s="48"/>
-      <c r="R47" s="48"/>
-      <c r="T47" s="52" t="s">
-        <v>142</v>
+      <c r="M47" s="52"/>
+      <c r="N47" s="52"/>
+      <c r="O47" s="52"/>
+      <c r="P47" s="52"/>
+      <c r="Q47" s="52"/>
+      <c r="R47" s="52"/>
+      <c r="T47" s="48" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C48" s="34" t="s">
-        <v>132</v>
-      </c>
-      <c r="D48" s="54" t="s">
-        <v>108</v>
-      </c>
-      <c r="E48" s="54"/>
-      <c r="F48" s="54"/>
-      <c r="G48" s="54"/>
-      <c r="H48" s="54"/>
-      <c r="I48" s="54"/>
-      <c r="J48" s="54"/>
-      <c r="L48" s="48" t="s">
-        <v>135</v>
-      </c>
-      <c r="M48" s="48"/>
-      <c r="N48" s="48"/>
-      <c r="O48" s="48"/>
-      <c r="P48" s="48"/>
-      <c r="Q48" s="48"/>
-      <c r="R48" s="48"/>
-      <c r="T48" s="52" t="s">
-        <v>143</v>
+        <v>128</v>
+      </c>
+      <c r="D48" s="50" t="s">
+        <v>104</v>
+      </c>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+      <c r="G48" s="50"/>
+      <c r="H48" s="50"/>
+      <c r="I48" s="50"/>
+      <c r="J48" s="50"/>
+      <c r="L48" s="52" t="s">
+        <v>131</v>
+      </c>
+      <c r="M48" s="52"/>
+      <c r="N48" s="52"/>
+      <c r="O48" s="52"/>
+      <c r="P48" s="52"/>
+      <c r="Q48" s="52"/>
+      <c r="R48" s="52"/>
+      <c r="T48" s="48" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C49" s="34" t="s">
-        <v>131</v>
-      </c>
-      <c r="D49" s="54" t="s">
-        <v>109</v>
-      </c>
-      <c r="E49" s="54"/>
-      <c r="F49" s="54"/>
-      <c r="G49" s="54"/>
-      <c r="H49" s="54"/>
-      <c r="I49" s="54"/>
-      <c r="J49" s="54"/>
-      <c r="L49" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="M49" s="48"/>
-      <c r="N49" s="48"/>
-      <c r="O49" s="48"/>
-      <c r="P49" s="48"/>
-      <c r="Q49" s="48"/>
-      <c r="R49" s="48"/>
-      <c r="T49" s="52" t="s">
-        <v>144</v>
+        <v>127</v>
+      </c>
+      <c r="D49" s="50" t="s">
+        <v>105</v>
+      </c>
+      <c r="E49" s="50"/>
+      <c r="F49" s="50"/>
+      <c r="G49" s="50"/>
+      <c r="H49" s="50"/>
+      <c r="I49" s="50"/>
+      <c r="J49" s="50"/>
+      <c r="L49" s="52" t="s">
+        <v>130</v>
+      </c>
+      <c r="M49" s="52"/>
+      <c r="N49" s="52"/>
+      <c r="O49" s="52"/>
+      <c r="P49" s="52"/>
+      <c r="Q49" s="52"/>
+      <c r="R49" s="52"/>
+      <c r="T49" s="48" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C50" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="D50" s="54" t="s">
-        <v>110</v>
-      </c>
-      <c r="E50" s="54"/>
-      <c r="F50" s="54"/>
-      <c r="G50" s="54"/>
-      <c r="H50" s="54"/>
-      <c r="I50" s="54"/>
-      <c r="J50" s="54"/>
-      <c r="L50" s="48" t="s">
-        <v>128</v>
-      </c>
-      <c r="M50" s="48"/>
-      <c r="N50" s="48"/>
-      <c r="O50" s="48"/>
-      <c r="P50" s="48"/>
-      <c r="Q50" s="48"/>
-      <c r="R50" s="48"/>
+        <v>129</v>
+      </c>
+      <c r="D50" s="50" t="s">
+        <v>106</v>
+      </c>
+      <c r="E50" s="50"/>
+      <c r="F50" s="50"/>
+      <c r="G50" s="50"/>
+      <c r="H50" s="50"/>
+      <c r="I50" s="50"/>
+      <c r="J50" s="50"/>
+      <c r="L50" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="M50" s="52"/>
+      <c r="N50" s="52"/>
+      <c r="O50" s="52"/>
+      <c r="P50" s="52"/>
+      <c r="Q50" s="52"/>
+      <c r="R50" s="52"/>
       <c r="T50" s="28" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" s="54" t="s">
-        <v>111</v>
-      </c>
-      <c r="E51" s="54"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="54"/>
-      <c r="H51" s="54"/>
-      <c r="I51" s="54"/>
-      <c r="J51" s="54"/>
-      <c r="L51" s="48" t="s">
-        <v>127</v>
-      </c>
-      <c r="M51" s="48"/>
-      <c r="N51" s="48"/>
-      <c r="O51" s="48"/>
-      <c r="P51" s="48"/>
-      <c r="Q51" s="48"/>
-      <c r="R51" s="48"/>
+        <v>129</v>
+      </c>
+      <c r="D51" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
+      <c r="L51" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="M51" s="52"/>
+      <c r="N51" s="52"/>
+      <c r="O51" s="52"/>
+      <c r="P51" s="52"/>
+      <c r="Q51" s="52"/>
+      <c r="R51" s="52"/>
       <c r="T51" s="28" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" s="50" t="s">
+        <v>108</v>
+      </c>
+      <c r="E52" s="50"/>
+      <c r="F52" s="50"/>
+      <c r="G52" s="50"/>
+      <c r="H52" s="50"/>
+      <c r="I52" s="50"/>
+      <c r="J52" s="50"/>
+      <c r="L52" s="52" t="s">
         <v>122</v>
       </c>
-      <c r="C52" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="D52" s="54" t="s">
-        <v>112</v>
-      </c>
-      <c r="E52" s="54"/>
-      <c r="F52" s="54"/>
-      <c r="G52" s="54"/>
-      <c r="H52" s="54"/>
-      <c r="I52" s="54"/>
-      <c r="J52" s="54"/>
-      <c r="L52" s="48" t="s">
-        <v>126</v>
-      </c>
-      <c r="M52" s="48"/>
-      <c r="N52" s="48"/>
-      <c r="O52" s="48"/>
-      <c r="P52" s="48"/>
-      <c r="Q52" s="48"/>
-      <c r="R52" s="48"/>
+      <c r="M52" s="52"/>
+      <c r="N52" s="52"/>
+      <c r="O52" s="52"/>
+      <c r="P52" s="52"/>
+      <c r="Q52" s="52"/>
+      <c r="R52" s="52"/>
       <c r="T52" s="28" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C53" s="34" t="s">
-        <v>133</v>
-      </c>
-      <c r="D53" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="E53" s="54"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="54"/>
-      <c r="H53" s="54"/>
-      <c r="I53" s="54"/>
-      <c r="J53" s="54"/>
-      <c r="L53" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="M53" s="48"/>
-      <c r="N53" s="48"/>
-      <c r="O53" s="48"/>
-      <c r="P53" s="48"/>
-      <c r="Q53" s="48"/>
-      <c r="R53" s="48"/>
+        <v>129</v>
+      </c>
+      <c r="D53" s="50" t="s">
+        <v>109</v>
+      </c>
+      <c r="E53" s="50"/>
+      <c r="F53" s="50"/>
+      <c r="G53" s="50"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="50"/>
+      <c r="J53" s="50"/>
+      <c r="L53" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="M53" s="52"/>
+      <c r="N53" s="52"/>
+      <c r="O53" s="52"/>
+      <c r="P53" s="52"/>
+      <c r="Q53" s="52"/>
+      <c r="R53" s="52"/>
       <c r="T53" s="34" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3216,7 +3250,7 @@
         <v>9</v>
       </c>
       <c r="L63" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M63" s="32" t="s">
         <v>9</v>
@@ -3233,6 +3267,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="L52:R52"/>
+    <mergeCell ref="L53:R53"/>
+    <mergeCell ref="L42:R42"/>
+    <mergeCell ref="L43:R43"/>
+    <mergeCell ref="L44:R44"/>
+    <mergeCell ref="L45:R45"/>
+    <mergeCell ref="L46:R46"/>
+    <mergeCell ref="L47:R47"/>
+    <mergeCell ref="L48:R48"/>
+    <mergeCell ref="L49:R49"/>
+    <mergeCell ref="L50:R50"/>
+    <mergeCell ref="L51:R51"/>
     <mergeCell ref="D52:J52"/>
     <mergeCell ref="D53:J53"/>
     <mergeCell ref="D42:J42"/>
@@ -3245,111 +3291,129 @@
     <mergeCell ref="D49:J49"/>
     <mergeCell ref="D50:J50"/>
     <mergeCell ref="D51:J51"/>
-    <mergeCell ref="L52:R52"/>
-    <mergeCell ref="L53:R53"/>
-    <mergeCell ref="L42:R42"/>
-    <mergeCell ref="L43:R43"/>
-    <mergeCell ref="L44:R44"/>
-    <mergeCell ref="L45:R45"/>
-    <mergeCell ref="L46:R46"/>
-    <mergeCell ref="L47:R47"/>
-    <mergeCell ref="L48:R48"/>
-    <mergeCell ref="L49:R49"/>
-    <mergeCell ref="L50:R50"/>
-    <mergeCell ref="L51:R51"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="E18 E14 E24:E26 E32:E35 E30 E20:E22 E3:E11 J13:K13 H13">
-    <cfRule type="cellIs" dxfId="20" priority="29" operator="equal">
+  <conditionalFormatting sqref="E18 E24:E26 E32:E35 E30 E20:E22 E3:E11 J13:K13 H13">
+    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63 D18 D24:D26 D32:D35 D30 D20:D22 D3:D11">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35">
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12">
+    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23">
     <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="D31">
     <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+  <conditionalFormatting sqref="D36">
     <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:G14">
-    <cfRule type="cellIs" dxfId="11" priority="13" operator="equal">
+  <conditionalFormatting sqref="D28">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+  <conditionalFormatting sqref="D13:G14">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63 D18 D14 D24:D26 D32:D35 D30 D20:D22 D3:D11">
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+  <conditionalFormatting sqref="D16:G17">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
-      <formula>"ja"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="7" priority="9" operator="equal">
-      <formula>"ja"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23">
+  <conditionalFormatting sqref="F37:F38">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D31">
+  <conditionalFormatting sqref="F29">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="F26">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
+  <conditionalFormatting sqref="F25">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"ja"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28">
+  <conditionalFormatting sqref="F8">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:G17">
+  <conditionalFormatting sqref="F3:F5">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
@@ -3594,15 +3658,15 @@
       <c r="B9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
       <c r="J9" s="3" t="s">
         <v>19</v>
       </c>
@@ -3688,15 +3752,15 @@
       <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="51"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="54"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="54"/>
+      <c r="I13" s="54"/>
       <c r="J13" s="3" t="s">
         <v>19</v>
       </c>
@@ -3709,15 +3773,15 @@
       <c r="B14" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="51"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="54"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
       <c r="J14" s="3" t="s">
         <v>19</v>
       </c>
@@ -3774,15 +3838,15 @@
       <c r="B17" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="54" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
       <c r="J17" s="3" t="s">
         <v>19</v>
       </c>
@@ -3795,15 +3859,15 @@
       <c r="B18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="51" t="s">
+      <c r="C18" s="54" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
       <c r="J18" s="3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
[ELAB-414] rework of 'Werkzeuge und Technologien'^9
</commit_message>
<xml_diff>
--- a/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
+++ b/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\tools-und-werkzeuge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05A5FCD-A2EC-447F-8801-A55D6D72C7BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1181B5-0885-4E30-8402-BA262113DF12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
   </bookViews>
@@ -787,12 +787,6 @@
     <t>Ignore</t>
   </si>
   <si>
-    <t>Log-Plattform</t>
-  </si>
-  <si>
-    <t>Tracing-Plattform</t>
-  </si>
-  <si>
     <t>Error-Tracking</t>
   </si>
   <si>
@@ -802,12 +796,6 @@
     <t>IM</t>
   </si>
   <si>
-    <t>APM-Plattform</t>
-  </si>
-  <si>
-    <t>Session-Replay-Dienst</t>
-  </si>
-  <si>
     <t>eingeschr.</t>
   </si>
   <si>
@@ -815,6 +803,18 @@
   </si>
   <si>
     <t>eing.</t>
+  </si>
+  <si>
+    <t>Session-Replay-Dienste</t>
+  </si>
+  <si>
+    <t>Log-Plattformen</t>
+  </si>
+  <si>
+    <t>APM-Plattformen</t>
+  </si>
+  <si>
+    <t>Distributed-Tracing-Systeme</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1750,7 @@
   <dimension ref="A1:T63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F3:F5"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1788,10 +1788,10 @@
         <v>73</v>
       </c>
       <c r="D1" s="44" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F1" s="44" t="s">
         <v>5</v>
@@ -1837,7 +1837,7 @@
     </row>
     <row r="2" spans="1:20" s="45" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B2" s="45" t="s">
         <v>152</v>
@@ -1872,7 +1872,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G3" s="30" t="s">
         <v>9</v>
@@ -1881,7 +1881,7 @@
         <v>9</v>
       </c>
       <c r="I3" s="35" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L3" s="37" t="s">
         <v>77</v>
@@ -1896,7 +1896,7 @@
         <v>9</v>
       </c>
       <c r="P3" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q3" s="30" t="s">
         <v>9</v>
@@ -1916,7 +1916,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G4" s="32" t="s">
         <v>9</v>
@@ -1940,7 +1940,7 @@
         <v>9</v>
       </c>
       <c r="P4" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q4" s="32" t="s">
         <v>9</v>
@@ -1963,7 +1963,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G5" s="32" t="s">
         <v>9</v>
@@ -1987,7 +1987,7 @@
         <v>9</v>
       </c>
       <c r="P5" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q5" s="32" t="s">
         <v>9</v>
@@ -2060,7 +2060,7 @@
         <v>77</v>
       </c>
       <c r="M7" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N7" s="38" t="s">
         <v>60</v>
@@ -2092,7 +2092,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G8" s="32" t="s">
         <v>9</v>
@@ -2116,7 +2116,7 @@
         <v>9</v>
       </c>
       <c r="P8" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q8" s="32" t="s">
         <v>9</v>
@@ -2157,7 +2157,7 @@
         <v>9</v>
       </c>
       <c r="P9" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q9" s="32" t="s">
         <v>9</v>
@@ -2180,7 +2180,7 @@
         <v>9</v>
       </c>
       <c r="M10" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N10" s="32" t="s">
         <v>9</v>
@@ -2189,7 +2189,7 @@
         <v>60</v>
       </c>
       <c r="P10" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q10" s="38" t="s">
         <v>60</v>
@@ -2204,7 +2204,7 @@
     <row r="11" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="42" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2212,16 +2212,16 @@
         <v>90</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G13" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I13" s="32" t="s">
         <v>9</v>
@@ -2230,7 +2230,7 @@
         <v>78</v>
       </c>
       <c r="M13" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N13" s="38" t="s">
         <v>60</v>
@@ -2253,16 +2253,16 @@
         <v>3</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E14" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G14" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I14" s="32" t="s">
         <v>9</v>
@@ -2271,7 +2271,7 @@
         <v>9</v>
       </c>
       <c r="M14" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N14" s="32" t="s">
         <v>9</v>
@@ -2280,7 +2280,7 @@
         <v>9</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q14" s="32" t="s">
         <v>9</v>
@@ -2297,13 +2297,13 @@
         <v>71</v>
       </c>
       <c r="I15" s="35" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L15" s="32" t="s">
         <v>9</v>
       </c>
       <c r="M15" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N15" s="32" t="s">
         <v>9</v>
@@ -2312,7 +2312,7 @@
         <v>9</v>
       </c>
       <c r="P15" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q15" s="38" t="s">
         <v>60</v>
@@ -2329,16 +2329,16 @@
         <v>80</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E16" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F16" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G16" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I16" s="32" t="s">
         <v>9</v>
@@ -2347,7 +2347,7 @@
         <v>78</v>
       </c>
       <c r="M16" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N16" s="32" t="s">
         <v>9</v>
@@ -2373,16 +2373,16 @@
         <v>91</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F17" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G17" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="I17" s="32" t="s">
         <v>9</v>
@@ -2391,7 +2391,7 @@
         <v>9</v>
       </c>
       <c r="M17" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N17" s="32" t="s">
         <v>9</v>
@@ -2400,7 +2400,7 @@
         <v>9</v>
       </c>
       <c r="P17" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q17" s="32" t="s">
         <v>9</v>
@@ -2415,7 +2415,7 @@
     <row r="18" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2429,7 +2429,7 @@
         <v>9</v>
       </c>
       <c r="M20" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N20" s="32" t="s">
         <v>9</v>
@@ -2461,7 +2461,7 @@
         <v>9</v>
       </c>
       <c r="M21" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="N21" s="32" t="s">
         <v>9</v>
@@ -2470,7 +2470,7 @@
         <v>60</v>
       </c>
       <c r="P21" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q21" s="38" t="s">
         <v>60</v>
@@ -2485,7 +2485,7 @@
     <row r="22" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:20" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:20" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G24" s="32" t="s">
         <v>9</v>
@@ -2511,7 +2511,7 @@
         <v>9</v>
       </c>
       <c r="P24" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q24" s="38" t="s">
         <v>60</v>
@@ -2525,7 +2525,7 @@
         <v>64</v>
       </c>
       <c r="F25" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G25" s="32" t="s">
         <v>9</v>
@@ -2557,7 +2557,7 @@
         <v>65</v>
       </c>
       <c r="F26" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G26" s="32" t="s">
         <v>9</v>
@@ -2639,7 +2639,7 @@
         <v>9</v>
       </c>
       <c r="P28" s="40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="Q28" s="38" t="s">
         <v>60</v>
@@ -2659,7 +2659,7 @@
         <v>9</v>
       </c>
       <c r="F29" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G29" s="32" t="s">
         <v>9</v>
@@ -2820,16 +2820,16 @@
         <v>88</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E37" s="39" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F37" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G37" s="39" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L37" s="39" t="s">
         <v>78</v>
@@ -2858,16 +2858,16 @@
         <v>89</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E38" s="39" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F38" s="39" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G38" s="39" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="L38" s="35" t="s">
         <v>77</v>

</xml_diff>

<commit_message>
[ELAB-432] adapt feedback from cwa
</commit_message>
<xml_diff>
--- a/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
+++ b/data/tools-und-werkzeuge/Tools-und-Werkzeuge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\bachelorarbeit\data\tools-und-werkzeuge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1181B5-0885-4E30-8402-BA262113DF12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76332453-9C3C-4357-A06C-CA663A179581}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{97483665-8731-4B46-80DA-A5AC37BBF732}"/>
   </bookViews>
@@ -1202,16 +1202,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1227,35 +1227,7 @@
     <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill>
@@ -1749,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65FA36FA-A460-4BBC-B832-96B5FC35BB7A}">
   <dimension ref="A1:T63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2720,8 +2692,8 @@
       <c r="P32" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q32" s="38" t="s">
-        <v>60</v>
+      <c r="Q32" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="R32" s="29" t="s">
         <v>150</v>
@@ -2758,8 +2730,8 @@
       <c r="P33" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q33" s="38" t="s">
-        <v>60</v>
+      <c r="Q33" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="R33" s="29" t="s">
         <v>150</v>
@@ -2796,8 +2768,8 @@
       <c r="P34" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="Q34" s="38" t="s">
-        <v>60</v>
+      <c r="Q34" s="32" t="s">
+        <v>9</v>
       </c>
       <c r="R34" s="31" t="s">
         <v>86</v>
@@ -2904,24 +2876,24 @@
       <c r="C42" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="D42" s="51" t="s">
+      <c r="D42" s="53" t="s">
         <v>98</v>
       </c>
-      <c r="E42" s="51"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="51"/>
-      <c r="L42" s="53" t="s">
+      <c r="E42" s="53"/>
+      <c r="F42" s="53"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="L42" s="51" t="s">
         <v>120</v>
       </c>
-      <c r="M42" s="53"/>
-      <c r="N42" s="53"/>
-      <c r="O42" s="53"/>
-      <c r="P42" s="53"/>
-      <c r="Q42" s="53"/>
-      <c r="R42" s="53"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="51"/>
+      <c r="O42" s="51"/>
+      <c r="P42" s="51"/>
+      <c r="Q42" s="51"/>
+      <c r="R42" s="51"/>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
@@ -2930,24 +2902,24 @@
       <c r="C43" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="D43" s="50" t="s">
+      <c r="D43" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
-      <c r="L43" s="52" t="s">
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
+      <c r="L43" s="50" t="s">
         <v>97</v>
       </c>
-      <c r="M43" s="52"/>
-      <c r="N43" s="52"/>
-      <c r="O43" s="52"/>
-      <c r="P43" s="52"/>
-      <c r="Q43" s="52"/>
-      <c r="R43" s="52"/>
+      <c r="M43" s="50"/>
+      <c r="N43" s="50"/>
+      <c r="O43" s="50"/>
+      <c r="P43" s="50"/>
+      <c r="Q43" s="50"/>
+      <c r="R43" s="50"/>
       <c r="T43" s="48" t="s">
         <v>134</v>
       </c>
@@ -2959,24 +2931,24 @@
       <c r="C44" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D44" s="50" t="s">
+      <c r="D44" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="50"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="50"/>
-      <c r="L44" s="52" t="s">
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
+      <c r="L44" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="M44" s="52"/>
-      <c r="N44" s="52"/>
-      <c r="O44" s="52"/>
-      <c r="P44" s="52"/>
-      <c r="Q44" s="52"/>
-      <c r="R44" s="52"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
+      <c r="R44" s="50"/>
       <c r="T44" s="48" t="s">
         <v>135</v>
       </c>
@@ -2988,24 +2960,24 @@
       <c r="C45" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D45" s="50" t="s">
+      <c r="D45" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
-      <c r="G45" s="50"/>
-      <c r="H45" s="50"/>
-      <c r="I45" s="50"/>
-      <c r="J45" s="50"/>
-      <c r="L45" s="52" t="s">
+      <c r="E45" s="52"/>
+      <c r="F45" s="52"/>
+      <c r="G45" s="52"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
+      <c r="L45" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="M45" s="52"/>
-      <c r="N45" s="52"/>
-      <c r="O45" s="52"/>
-      <c r="P45" s="52"/>
-      <c r="Q45" s="52"/>
-      <c r="R45" s="52"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="50"/>
+      <c r="P45" s="50"/>
+      <c r="Q45" s="50"/>
+      <c r="R45" s="50"/>
       <c r="T45" s="48" t="s">
         <v>136</v>
       </c>
@@ -3017,24 +2989,24 @@
       <c r="C46" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D46" s="50" t="s">
+      <c r="D46" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
-      <c r="G46" s="50"/>
-      <c r="H46" s="50"/>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
-      <c r="L46" s="52" t="s">
+      <c r="E46" s="52"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="52"/>
+      <c r="H46" s="52"/>
+      <c r="I46" s="52"/>
+      <c r="J46" s="52"/>
+      <c r="L46" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="M46" s="52"/>
-      <c r="N46" s="52"/>
-      <c r="O46" s="52"/>
-      <c r="P46" s="52"/>
-      <c r="Q46" s="52"/>
-      <c r="R46" s="52"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="50"/>
+      <c r="P46" s="50"/>
+      <c r="Q46" s="50"/>
+      <c r="R46" s="50"/>
       <c r="T46" s="48" t="s">
         <v>137</v>
       </c>
@@ -3046,24 +3018,24 @@
       <c r="C47" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D47" s="50" t="s">
+      <c r="D47" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="50"/>
-      <c r="H47" s="50"/>
-      <c r="I47" s="50"/>
-      <c r="J47" s="50"/>
-      <c r="L47" s="52" t="s">
+      <c r="E47" s="52"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="52"/>
+      <c r="H47" s="52"/>
+      <c r="I47" s="52"/>
+      <c r="J47" s="52"/>
+      <c r="L47" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="M47" s="52"/>
-      <c r="N47" s="52"/>
-      <c r="O47" s="52"/>
-      <c r="P47" s="52"/>
-      <c r="Q47" s="52"/>
-      <c r="R47" s="52"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="50"/>
+      <c r="P47" s="50"/>
+      <c r="Q47" s="50"/>
+      <c r="R47" s="50"/>
       <c r="T47" s="48" t="s">
         <v>138</v>
       </c>
@@ -3075,24 +3047,24 @@
       <c r="C48" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="D48" s="50" t="s">
+      <c r="D48" s="52" t="s">
         <v>104</v>
       </c>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="50"/>
-      <c r="H48" s="50"/>
-      <c r="I48" s="50"/>
-      <c r="J48" s="50"/>
-      <c r="L48" s="52" t="s">
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
+      <c r="H48" s="52"/>
+      <c r="I48" s="52"/>
+      <c r="J48" s="52"/>
+      <c r="L48" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="M48" s="52"/>
-      <c r="N48" s="52"/>
-      <c r="O48" s="52"/>
-      <c r="P48" s="52"/>
-      <c r="Q48" s="52"/>
-      <c r="R48" s="52"/>
+      <c r="M48" s="50"/>
+      <c r="N48" s="50"/>
+      <c r="O48" s="50"/>
+      <c r="P48" s="50"/>
+      <c r="Q48" s="50"/>
+      <c r="R48" s="50"/>
       <c r="T48" s="48" t="s">
         <v>139</v>
       </c>
@@ -3104,24 +3076,24 @@
       <c r="C49" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="D49" s="50" t="s">
+      <c r="D49" s="52" t="s">
         <v>105</v>
       </c>
-      <c r="E49" s="50"/>
-      <c r="F49" s="50"/>
-      <c r="G49" s="50"/>
-      <c r="H49" s="50"/>
-      <c r="I49" s="50"/>
-      <c r="J49" s="50"/>
-      <c r="L49" s="52" t="s">
+      <c r="E49" s="52"/>
+      <c r="F49" s="52"/>
+      <c r="G49" s="52"/>
+      <c r="H49" s="52"/>
+      <c r="I49" s="52"/>
+      <c r="J49" s="52"/>
+      <c r="L49" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="M49" s="52"/>
-      <c r="N49" s="52"/>
-      <c r="O49" s="52"/>
-      <c r="P49" s="52"/>
-      <c r="Q49" s="52"/>
-      <c r="R49" s="52"/>
+      <c r="M49" s="50"/>
+      <c r="N49" s="50"/>
+      <c r="O49" s="50"/>
+      <c r="P49" s="50"/>
+      <c r="Q49" s="50"/>
+      <c r="R49" s="50"/>
       <c r="T49" s="48" t="s">
         <v>140</v>
       </c>
@@ -3133,24 +3105,24 @@
       <c r="C50" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="D50" s="50" t="s">
+      <c r="D50" s="52" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="50"/>
-      <c r="F50" s="50"/>
-      <c r="G50" s="50"/>
-      <c r="H50" s="50"/>
-      <c r="I50" s="50"/>
-      <c r="J50" s="50"/>
-      <c r="L50" s="52" t="s">
+      <c r="E50" s="52"/>
+      <c r="F50" s="52"/>
+      <c r="G50" s="52"/>
+      <c r="H50" s="52"/>
+      <c r="I50" s="52"/>
+      <c r="J50" s="52"/>
+      <c r="L50" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="M50" s="52"/>
-      <c r="N50" s="52"/>
-      <c r="O50" s="52"/>
-      <c r="P50" s="52"/>
-      <c r="Q50" s="52"/>
-      <c r="R50" s="52"/>
+      <c r="M50" s="50"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="50"/>
+      <c r="P50" s="50"/>
+      <c r="Q50" s="50"/>
+      <c r="R50" s="50"/>
       <c r="T50" s="28" t="s">
         <v>142</v>
       </c>
@@ -3162,24 +3134,24 @@
       <c r="C51" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="D51" s="50" t="s">
+      <c r="D51" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="50"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="50"/>
-      <c r="J51" s="50"/>
-      <c r="L51" s="52" t="s">
+      <c r="E51" s="52"/>
+      <c r="F51" s="52"/>
+      <c r="G51" s="52"/>
+      <c r="H51" s="52"/>
+      <c r="I51" s="52"/>
+      <c r="J51" s="52"/>
+      <c r="L51" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="M51" s="52"/>
-      <c r="N51" s="52"/>
-      <c r="O51" s="52"/>
-      <c r="P51" s="52"/>
-      <c r="Q51" s="52"/>
-      <c r="R51" s="52"/>
+      <c r="M51" s="50"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="50"/>
+      <c r="P51" s="50"/>
+      <c r="Q51" s="50"/>
+      <c r="R51" s="50"/>
       <c r="T51" s="28" t="s">
         <v>141</v>
       </c>
@@ -3191,24 +3163,24 @@
       <c r="C52" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="D52" s="50" t="s">
+      <c r="D52" s="52" t="s">
         <v>108</v>
       </c>
-      <c r="E52" s="50"/>
-      <c r="F52" s="50"/>
-      <c r="G52" s="50"/>
-      <c r="H52" s="50"/>
-      <c r="I52" s="50"/>
-      <c r="J52" s="50"/>
-      <c r="L52" s="52" t="s">
+      <c r="E52" s="52"/>
+      <c r="F52" s="52"/>
+      <c r="G52" s="52"/>
+      <c r="H52" s="52"/>
+      <c r="I52" s="52"/>
+      <c r="J52" s="52"/>
+      <c r="L52" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="M52" s="52"/>
-      <c r="N52" s="52"/>
-      <c r="O52" s="52"/>
-      <c r="P52" s="52"/>
-      <c r="Q52" s="52"/>
-      <c r="R52" s="52"/>
+      <c r="M52" s="50"/>
+      <c r="N52" s="50"/>
+      <c r="O52" s="50"/>
+      <c r="P52" s="50"/>
+      <c r="Q52" s="50"/>
+      <c r="R52" s="50"/>
       <c r="T52" s="28" t="s">
         <v>143</v>
       </c>
@@ -3220,24 +3192,24 @@
       <c r="C53" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="D53" s="50" t="s">
+      <c r="D53" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="E53" s="50"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="50"/>
-      <c r="H53" s="50"/>
-      <c r="I53" s="50"/>
-      <c r="J53" s="50"/>
-      <c r="L53" s="52" t="s">
+      <c r="E53" s="52"/>
+      <c r="F53" s="52"/>
+      <c r="G53" s="52"/>
+      <c r="H53" s="52"/>
+      <c r="I53" s="52"/>
+      <c r="J53" s="52"/>
+      <c r="L53" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="M53" s="52"/>
-      <c r="N53" s="52"/>
-      <c r="O53" s="52"/>
-      <c r="P53" s="52"/>
-      <c r="Q53" s="52"/>
-      <c r="R53" s="52"/>
+      <c r="M53" s="50"/>
+      <c r="N53" s="50"/>
+      <c r="O53" s="50"/>
+      <c r="P53" s="50"/>
+      <c r="Q53" s="50"/>
+      <c r="R53" s="50"/>
       <c r="T53" s="34" t="s">
         <v>144</v>
       </c>
@@ -3267,6 +3239,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D52:J52"/>
+    <mergeCell ref="D53:J53"/>
+    <mergeCell ref="D42:J42"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="D44:J44"/>
+    <mergeCell ref="D45:J45"/>
+    <mergeCell ref="D46:J46"/>
+    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="D48:J48"/>
+    <mergeCell ref="D49:J49"/>
+    <mergeCell ref="D50:J50"/>
+    <mergeCell ref="D51:J51"/>
     <mergeCell ref="L52:R52"/>
     <mergeCell ref="L53:R53"/>
     <mergeCell ref="L42:R42"/>
@@ -3279,102 +3263,90 @@
     <mergeCell ref="L49:R49"/>
     <mergeCell ref="L50:R50"/>
     <mergeCell ref="L51:R51"/>
-    <mergeCell ref="D52:J52"/>
-    <mergeCell ref="D53:J53"/>
-    <mergeCell ref="D42:J42"/>
-    <mergeCell ref="D43:J43"/>
-    <mergeCell ref="D44:J44"/>
-    <mergeCell ref="D45:J45"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="D47:J47"/>
-    <mergeCell ref="D48:J48"/>
-    <mergeCell ref="D49:J49"/>
-    <mergeCell ref="D50:J50"/>
-    <mergeCell ref="D51:J51"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <conditionalFormatting sqref="E18 E24:E26 E32:E35 E30 E20:E22 E3:E11 J13:K13 H13">
-    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="39" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="36" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="34" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="18" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="27" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="cellIs" dxfId="19" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63 D18 D24:D26 D32:D35 D30 D20:D22 D3:D11">
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="20" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="cellIs" dxfId="15" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="13" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13:G14">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>"ja"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>